<commit_message>
started pseudo driver as chardriver
</commit_message>
<xml_diff>
--- a/short_notes.xlsx
+++ b/short_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="interview preparation" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,14 +15,14 @@
     <sheet name="shell concepts" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="embedded_linux" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="kernel_programming" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="linux_device_driver" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="651">
   <si>
     <t>Sr No</t>
   </si>
@@ -3797,15 +3797,13 @@
     <t>ktype</t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 - Kobjects are associated with a specific type, called a ktype.
 - Ktypes are represented by struct kobj_type and defined in &lt;linux/kobject.h&gt; :
 - Ktypes have the simple job of describing default behavior for a family of kobjects.
 - Instead of each kobject defining its own behavior, the behavior is stored in a ktype, and kobjects of the same “type” point at the same ktype structure, thus sharing the same behavior.
 - The release pointer points to the deconstructor called when a kobject’s reference count reaches zero.This function is responsible for freeing any memory associated with this kobject and otherwise cleaning up.
 </t>
-    </r>
   </si>
   <si>
     <t>
@@ -3854,8 +3852,7 @@
     <t>Managing and Manipulating Kobjects</t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 - The first step in using a kobject is declaring and initializing it. this is done using following which is declared in &lt;linux/kobject.h&gt; :
     struct kobject * kobject_create(void);
 - After initialization, the kobject’s reference count is set to one. So long as the reference count is nonzero, the object continues to exist in memory and is said to be pinned.
@@ -3864,7 +3861,6 @@
     struct kobject * kobject_get(struct kobject *kobj); // increment reference count (getting)
     void kobject_put(struct kobject *kobj); // decrement reference count (putting)
 </t>
-    </r>
   </si>
   <si>
     <t>sysfs</t>
@@ -3945,8 +3941,7 @@
 </t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 - default attributes
     The attribute structure is defined in &lt;linux/sysfs.h&gt; :
     /* attribute structure - attributes map kernel data to a sysfs file */
@@ -3963,7 +3958,6 @@
         ssize_t (*store) (struct kobject *kobj, struct attribute *attr, const char *buffer, size_t size);
     };
 </t>
-    </r>
   </si>
   <si>
     <t>The Kernel Events Layer</t>
@@ -3979,6 +3973,210 @@
     - The first parameter specifies the kobject emitting this signal.
     - The second parameter specifies the action or verb describing this signal.The actual kernel event contains a string that maps to the provided enum kobject_action value.
 - This and related functions are defined in lib/kobject_uevent.c and declared in &lt;linux/kobject.h&gt; .
+</t>
+  </si>
+  <si>
+    <t>Char Drivers</t>
+  </si>
+  <si>
+    <t>Major and Minor Numbers</t>
+  </si>
+  <si>
+    <t>
+- the major number identifies the driver associated with the device.
+- The minor number is used by the kernel to determine exactly which device is being referred to.
+</t>
+  </si>
+  <si>
+    <t>The Internal Representation of Device Numbers</t>
+  </si>
+  <si>
+    <t>
+- Within the kernel, the dev_t type (defined in &lt;linux/types.h&gt;) is used to hold device numbers—both the major and minor parts.
+- To obtain the major or minor parts of a dev_t , use:
+    MAJOR(dev_t dev);
+    MINOR(dev_t dev);
+- If, instead, you have the major and minor numbers and need to turn them into a dev_t ,use:
+    MKDEV(int major, int minor);
+</t>
+  </si>
+  <si>
+    <t>Allocating and Freeing Device Numbers</t>
+  </si>
+  <si>
+    <t>
+- One of the first things your driver will need to do when setting up a char device is to obtain one or more device numbers to work with. 
+- The necessary function for this task is register_chrdev_region, which is declared in &lt;linux/fs.h&gt;:
+    int register_chrdev_region(dev_t first, unsigned int count, char *name);
+    - first is the beginning device number of the range you would like to allocate. The minor number portion of first is often 0.
+    - count is the total number of contiguous device numbers you are requesting.
+    - name is the name of the device that should be associated with this number range; it will appear in /proc/devices and sysfs
+    - the return value from register_chrdev_region will be 0 if the allocation was successfully performed. In case of error, a negative error code will be returned.
+- The kernel will allocate a major number for you on the fly, by using a function:
+    int alloc_chrdev_region(dev_t *dev, unsigned int firstminor, unsigned int count, char *name);
+    - With this function, dev is an output-only parameter that will, on successful completion, hold the first number in your allocated range.
+    - firstminor should be the requested first minor number to use; it is usually 0.
+- Regardless of how you allocate your device numbers, you should free them when they are no longer in use. Device numbers are freed with:
+    void unregister_chrdev_region(dev_t first, unsigned int count);
+- The disadvantage of dynamic assignment is that you can’t create the device nodes in advance, because the major number assigned to your module will vary. 
+- For normal use of the driver, this is hardly a problem, because once the number has been assigned, you can read it from /proc/devices.
+</t>
+  </si>
+  <si>
+    <t>Some Important Data Structures</t>
+  </si>
+  <si>
+    <t>
+- Most of the fundamental driver operations involve three important kernel data structures, called file_operations , file ,and inode .
+- File Operations
+- we have reserved some device numbers for our use, but we have not yet con nected any of our driver’s operations to those numbers. 
+- The file_operations structure is how a char driver sets up this connection.
+- The structure, defined in &lt;linux/fs.h&gt;, is a collection of function pointers.
+- Each field in the structure must point to the function in the driver that implements a specific operation, or be left NULL for unsupported operations.
+- The file Structure
+- struct file , defined in &lt;linux/fs.h&gt;, is the second most important data structure used in device drivers.
+- The file structure represents an open file. (It is not specific to device drivers; every open file in the system has an associated struct file in kernel space.) 
+- It is created by the kernel on open and is passed to any function that operates on the file, until the last close. After all instances of the file are closed, the kernel releases the data structure.
+- The inode Structure
+- The inode structure is used by the kernel internally to represent files. Therefore, it is different from the file structure that represents an open file descriptor.
+- There can be numerous file structures representing multiple open descriptors on a single file, but they all point to a single inode structure.
+- The inode structure contains a great deal of information about the file. As a general rule, only two fields of this structure are of interest for writing driver code:
+    dev_t i_rdev;
+    For inodes that represent device files, this field contains the actual device number.
+    struct cdev *i_cdev;
+    struct cdev is the kernel’s internal structure that represents char devices; this field contains a pointer to that structure when the inode refers to a char device file.
+</t>
+  </si>
+  <si>
+    <t>Char Device Registration</t>
+  </si>
+  <si>
+    <t>
+- the kernel uses structures of type struct cdev to represent char devices internally. 
+- Before the kernel invokes your device’s operations, you must allocate and register one or more of these structures.
+- To do so, your code should include &lt;linux/cdev.h&gt;
+- There are two ways of allocating and initializing one of these structures. If you wish to obtain a standalone cdev structure at runtime, 
+- you may do so with code such as:
+    struct cdev *my_cdev = cdev_alloc( );
+    my_cdev-&gt;ops = &amp;my_fops;
+- you should initialize the structure that you have already allocated with:
+    void cdev_init(struct cdev *cdev, struct file_operations *fops);
+    struct cdev *c_dev = kmalloc();
+    cdev_init(c_dev, fops);
+- Either way, there is one other struct cdev field that you need to initialize. Like the file_operations structure, struct cdev has an owner field that should be set to THIS_MODULE .
+- Once the cdev structure is set up, the final step is to tell the kernel about it with a call to:
+    int cdev_add(struct cdev *dev, dev_t num, unsigned int count);
+    - dev is the cdev structure, 
+    - num is the first device number to which this device responds
+    - count is the number of device numbers that should be associated with the device.
+    - this call can fail. If it returns a negative error code, your device has not been added to the system.
+    - You should not call cdev_add until your driver is completely ready to handle operations on the device.
+- To remove a char device from the system, call:
+    void cdev_del(struct cdev *dev);
+    - you should not access the cdev structure after passing it to cdev_del.
+</t>
+  </si>
+  <si>
+    <t>
+struct scull_dev {
+    struct scull_qset *data; /* Pointer to first quantum set */
+    int quantum; /* the current quantum size */
+    int qset; /* the current array size */
+    unsigned long size; /* amount of data stored here */
+    unsigned int access_key; /* used by sculluid and scullpriv */
+    struct semaphore sem; /* mutual exclusion semaphore */
+    struct cdev cdev; /* Char device structure */
+};
+static void scull_setup_cdev(struct scull_dev *dev, int index)
+{
+    int err, devno = MKDEV(scull_major, scull_minor + index);
+    cdev_init(&amp;dev-&gt;cdev, &amp;scull_fops);
+    dev-&gt;cdev.owner = THIS_MODULE;
+    dev-&gt;cdev.ops = &amp;scull_fops;
+    err = cdev_add (&amp;dev-&gt;cdev, devno, 1);
+    /* Fail gracefully if need be */
+    if (err)
+        printk(KERN_NOTICE "Error %d adding scull%d", err, index);
+}
+</t>
+  </si>
+  <si>
+    <t>open and release method</t>
+  </si>
+  <si>
+    <t>
+- Open method
+- The open method is provided for a driver to do any initialization in preparation for later operations. 
+- In most drivers, open should perform the following tasks:
+    • Check for device-specific errors (such as device-not-ready or similar hardware problems)
+    • Initialize the device if it is being opened for the first time
+    • Update the f_op pointer, if necessary
+    • Allocate and fill any data structure to be put in filp-&gt;private_data
+- The first order of business, however, is usually to identify which device is being opened. 
+- Remember that the prototype for the open method is:
+    int (*open)(struct inode *inode, struct file *filp);
+    • The inode argument has the information we need in the form of its i_cdev field, which contains the cdev structure we set up before.
+- The only problem is that we do not normally want the cdev structure itself, we want the scull_dev structure that contains that cdev structure.
+- which can get in the form of the container_of macro, defined in &lt;linux/kernel.h&gt;:
+    container_of(pointer, container_type, container_field);
+    - This macro takes a pointer to a field of type container_field , 
+    - within a structure of type container_type
+    - returns a pointer to the containing structure. 
+- In scull_open, this macro is used to find the appropriate device structure:
+    struct scull_dev *dev; /* device information */
+    dev = container_of(inode-&gt;i_cdev, struct scull_dev, cdev);
+    filp-&gt;private_data = dev; /* for other methods */
+</t>
+  </si>
+  <si>
+    <r>
+      <t>
+int scull_open(struct inode *inode, struct file *filp)
+{
+    struct scull_dev *dev; /* device information */
+    dev = container_of(inode-&gt;i_cdev, struct scull_dev, cdev);
+    filp-&gt;private_data = dev; /* for other methods */
+    /* now trim to 0 the length of the device if open was write-only */
+    if ( (filp-&gt;f_flags &amp; O_ACCMODE) = = O_WRONLY) {
+        scull_trim(dev); /* ignore errors */
+    }
+    return 0;
+    /* success */
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <t>
+- The release Method
+- The role of the release method is the reverse of open. Sometimes you’ll find that the method implementation is called device_close instead of device_release . 
+- Either way, the device method should perform the following tasks:
+• Deallocate anything that open allocated in filp-&gt;private_data
+• Shut down the device on last close
+</t>
+  </si>
+  <si>
+    <t>read and write</t>
+  </si>
+  <si>
+    <t>    
+- The read and write methods both perform a similar task, that is, copying data from and to application code.
+    ssize_t read(struct file *filp, char __user *buff, size_t count, loff_t *offp);
+    ssize_t write(struct file *filp, const char __user *buff, size_t count, loff_t *offp);
+    - filp is the file pointer and 
+    - count is the size of the requested data transfer. 
+    - The buff argument points to the user buffer holding the data to be written or the empty buffer where the newly read data should be placed. 
+    - Finally, offp is a pointer to a “long offset type” object that indicates the file position the user is accessing.
+    - Both the read and write methods return a negative value if an error occurs. 
+    - A return value greater than or equal to 0, instead, tells the calling program how many bytes have been successfully transferred. 
+    - If some data is transferred correctly and then an error happens, the return value must be the count of bytes successfully transferred.
+- your driver must be able to access the user-space buffer in order to get its job done. This access must always be performed by special, kernel-supplied functions, however, in order to be safe. We introduce some of those functions (which are defined in &lt;asm/uaccess.h&gt;)
+    unsigned long copy_to_user(void __user *to, const void *from, unsigned long count);
+    unsigned long copy_from_user(void *to, const void __user *from, unsigned long count);
+    - The role of the two functions is not limited to copying data to and from user-space: they also check whether the user space pointer is valid. 
+    - If the pointer is invalid, no copy is performed; if an invalid address is encountered during the copy, on the other hand, only part of the data is copied. In both cases, the return value is the amount of memory still to be copied.
+- Whatever the amount of data the methods transfer, they should generally update the file position at *offp to represent the current file position after successful completion of the system call. 
+- The kernel then propagates the file position change back into the file structure when appropriate.
 </t>
   </si>
 </sst>
@@ -4329,8 +4527,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -6611,21 +6809,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F141"/>
+  <dimension ref="1:141"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="6.4234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="38" width="23.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="38" width="28.8520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="80.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="38" width="65.7142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="38" width="32.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="38" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="34" width="6.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="35" width="23.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="35" width="28.8520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="80.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="65.7142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="32.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6648,6 +6846,1024 @@
       <c r="F2" s="36" t="s">
         <v>6</v>
       </c>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
+      <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
+      <c r="IX2" s="0"/>
+      <c r="IY2" s="0"/>
+      <c r="IZ2" s="0"/>
+      <c r="JA2" s="0"/>
+      <c r="JB2" s="0"/>
+      <c r="JC2" s="0"/>
+      <c r="JD2" s="0"/>
+      <c r="JE2" s="0"/>
+      <c r="JF2" s="0"/>
+      <c r="JG2" s="0"/>
+      <c r="JH2" s="0"/>
+      <c r="JI2" s="0"/>
+      <c r="JJ2" s="0"/>
+      <c r="JK2" s="0"/>
+      <c r="JL2" s="0"/>
+      <c r="JM2" s="0"/>
+      <c r="JN2" s="0"/>
+      <c r="JO2" s="0"/>
+      <c r="JP2" s="0"/>
+      <c r="JQ2" s="0"/>
+      <c r="JR2" s="0"/>
+      <c r="JS2" s="0"/>
+      <c r="JT2" s="0"/>
+      <c r="JU2" s="0"/>
+      <c r="JV2" s="0"/>
+      <c r="JW2" s="0"/>
+      <c r="JX2" s="0"/>
+      <c r="JY2" s="0"/>
+      <c r="JZ2" s="0"/>
+      <c r="KA2" s="0"/>
+      <c r="KB2" s="0"/>
+      <c r="KC2" s="0"/>
+      <c r="KD2" s="0"/>
+      <c r="KE2" s="0"/>
+      <c r="KF2" s="0"/>
+      <c r="KG2" s="0"/>
+      <c r="KH2" s="0"/>
+      <c r="KI2" s="0"/>
+      <c r="KJ2" s="0"/>
+      <c r="KK2" s="0"/>
+      <c r="KL2" s="0"/>
+      <c r="KM2" s="0"/>
+      <c r="KN2" s="0"/>
+      <c r="KO2" s="0"/>
+      <c r="KP2" s="0"/>
+      <c r="KQ2" s="0"/>
+      <c r="KR2" s="0"/>
+      <c r="KS2" s="0"/>
+      <c r="KT2" s="0"/>
+      <c r="KU2" s="0"/>
+      <c r="KV2" s="0"/>
+      <c r="KW2" s="0"/>
+      <c r="KX2" s="0"/>
+      <c r="KY2" s="0"/>
+      <c r="KZ2" s="0"/>
+      <c r="LA2" s="0"/>
+      <c r="LB2" s="0"/>
+      <c r="LC2" s="0"/>
+      <c r="LD2" s="0"/>
+      <c r="LE2" s="0"/>
+      <c r="LF2" s="0"/>
+      <c r="LG2" s="0"/>
+      <c r="LH2" s="0"/>
+      <c r="LI2" s="0"/>
+      <c r="LJ2" s="0"/>
+      <c r="LK2" s="0"/>
+      <c r="LL2" s="0"/>
+      <c r="LM2" s="0"/>
+      <c r="LN2" s="0"/>
+      <c r="LO2" s="0"/>
+      <c r="LP2" s="0"/>
+      <c r="LQ2" s="0"/>
+      <c r="LR2" s="0"/>
+      <c r="LS2" s="0"/>
+      <c r="LT2" s="0"/>
+      <c r="LU2" s="0"/>
+      <c r="LV2" s="0"/>
+      <c r="LW2" s="0"/>
+      <c r="LX2" s="0"/>
+      <c r="LY2" s="0"/>
+      <c r="LZ2" s="0"/>
+      <c r="MA2" s="0"/>
+      <c r="MB2" s="0"/>
+      <c r="MC2" s="0"/>
+      <c r="MD2" s="0"/>
+      <c r="ME2" s="0"/>
+      <c r="MF2" s="0"/>
+      <c r="MG2" s="0"/>
+      <c r="MH2" s="0"/>
+      <c r="MI2" s="0"/>
+      <c r="MJ2" s="0"/>
+      <c r="MK2" s="0"/>
+      <c r="ML2" s="0"/>
+      <c r="MM2" s="0"/>
+      <c r="MN2" s="0"/>
+      <c r="MO2" s="0"/>
+      <c r="MP2" s="0"/>
+      <c r="MQ2" s="0"/>
+      <c r="MR2" s="0"/>
+      <c r="MS2" s="0"/>
+      <c r="MT2" s="0"/>
+      <c r="MU2" s="0"/>
+      <c r="MV2" s="0"/>
+      <c r="MW2" s="0"/>
+      <c r="MX2" s="0"/>
+      <c r="MY2" s="0"/>
+      <c r="MZ2" s="0"/>
+      <c r="NA2" s="0"/>
+      <c r="NB2" s="0"/>
+      <c r="NC2" s="0"/>
+      <c r="ND2" s="0"/>
+      <c r="NE2" s="0"/>
+      <c r="NF2" s="0"/>
+      <c r="NG2" s="0"/>
+      <c r="NH2" s="0"/>
+      <c r="NI2" s="0"/>
+      <c r="NJ2" s="0"/>
+      <c r="NK2" s="0"/>
+      <c r="NL2" s="0"/>
+      <c r="NM2" s="0"/>
+      <c r="NN2" s="0"/>
+      <c r="NO2" s="0"/>
+      <c r="NP2" s="0"/>
+      <c r="NQ2" s="0"/>
+      <c r="NR2" s="0"/>
+      <c r="NS2" s="0"/>
+      <c r="NT2" s="0"/>
+      <c r="NU2" s="0"/>
+      <c r="NV2" s="0"/>
+      <c r="NW2" s="0"/>
+      <c r="NX2" s="0"/>
+      <c r="NY2" s="0"/>
+      <c r="NZ2" s="0"/>
+      <c r="OA2" s="0"/>
+      <c r="OB2" s="0"/>
+      <c r="OC2" s="0"/>
+      <c r="OD2" s="0"/>
+      <c r="OE2" s="0"/>
+      <c r="OF2" s="0"/>
+      <c r="OG2" s="0"/>
+      <c r="OH2" s="0"/>
+      <c r="OI2" s="0"/>
+      <c r="OJ2" s="0"/>
+      <c r="OK2" s="0"/>
+      <c r="OL2" s="0"/>
+      <c r="OM2" s="0"/>
+      <c r="ON2" s="0"/>
+      <c r="OO2" s="0"/>
+      <c r="OP2" s="0"/>
+      <c r="OQ2" s="0"/>
+      <c r="OR2" s="0"/>
+      <c r="OS2" s="0"/>
+      <c r="OT2" s="0"/>
+      <c r="OU2" s="0"/>
+      <c r="OV2" s="0"/>
+      <c r="OW2" s="0"/>
+      <c r="OX2" s="0"/>
+      <c r="OY2" s="0"/>
+      <c r="OZ2" s="0"/>
+      <c r="PA2" s="0"/>
+      <c r="PB2" s="0"/>
+      <c r="PC2" s="0"/>
+      <c r="PD2" s="0"/>
+      <c r="PE2" s="0"/>
+      <c r="PF2" s="0"/>
+      <c r="PG2" s="0"/>
+      <c r="PH2" s="0"/>
+      <c r="PI2" s="0"/>
+      <c r="PJ2" s="0"/>
+      <c r="PK2" s="0"/>
+      <c r="PL2" s="0"/>
+      <c r="PM2" s="0"/>
+      <c r="PN2" s="0"/>
+      <c r="PO2" s="0"/>
+      <c r="PP2" s="0"/>
+      <c r="PQ2" s="0"/>
+      <c r="PR2" s="0"/>
+      <c r="PS2" s="0"/>
+      <c r="PT2" s="0"/>
+      <c r="PU2" s="0"/>
+      <c r="PV2" s="0"/>
+      <c r="PW2" s="0"/>
+      <c r="PX2" s="0"/>
+      <c r="PY2" s="0"/>
+      <c r="PZ2" s="0"/>
+      <c r="QA2" s="0"/>
+      <c r="QB2" s="0"/>
+      <c r="QC2" s="0"/>
+      <c r="QD2" s="0"/>
+      <c r="QE2" s="0"/>
+      <c r="QF2" s="0"/>
+      <c r="QG2" s="0"/>
+      <c r="QH2" s="0"/>
+      <c r="QI2" s="0"/>
+      <c r="QJ2" s="0"/>
+      <c r="QK2" s="0"/>
+      <c r="QL2" s="0"/>
+      <c r="QM2" s="0"/>
+      <c r="QN2" s="0"/>
+      <c r="QO2" s="0"/>
+      <c r="QP2" s="0"/>
+      <c r="QQ2" s="0"/>
+      <c r="QR2" s="0"/>
+      <c r="QS2" s="0"/>
+      <c r="QT2" s="0"/>
+      <c r="QU2" s="0"/>
+      <c r="QV2" s="0"/>
+      <c r="QW2" s="0"/>
+      <c r="QX2" s="0"/>
+      <c r="QY2" s="0"/>
+      <c r="QZ2" s="0"/>
+      <c r="RA2" s="0"/>
+      <c r="RB2" s="0"/>
+      <c r="RC2" s="0"/>
+      <c r="RD2" s="0"/>
+      <c r="RE2" s="0"/>
+      <c r="RF2" s="0"/>
+      <c r="RG2" s="0"/>
+      <c r="RH2" s="0"/>
+      <c r="RI2" s="0"/>
+      <c r="RJ2" s="0"/>
+      <c r="RK2" s="0"/>
+      <c r="RL2" s="0"/>
+      <c r="RM2" s="0"/>
+      <c r="RN2" s="0"/>
+      <c r="RO2" s="0"/>
+      <c r="RP2" s="0"/>
+      <c r="RQ2" s="0"/>
+      <c r="RR2" s="0"/>
+      <c r="RS2" s="0"/>
+      <c r="RT2" s="0"/>
+      <c r="RU2" s="0"/>
+      <c r="RV2" s="0"/>
+      <c r="RW2" s="0"/>
+      <c r="RX2" s="0"/>
+      <c r="RY2" s="0"/>
+      <c r="RZ2" s="0"/>
+      <c r="SA2" s="0"/>
+      <c r="SB2" s="0"/>
+      <c r="SC2" s="0"/>
+      <c r="SD2" s="0"/>
+      <c r="SE2" s="0"/>
+      <c r="SF2" s="0"/>
+      <c r="SG2" s="0"/>
+      <c r="SH2" s="0"/>
+      <c r="SI2" s="0"/>
+      <c r="SJ2" s="0"/>
+      <c r="SK2" s="0"/>
+      <c r="SL2" s="0"/>
+      <c r="SM2" s="0"/>
+      <c r="SN2" s="0"/>
+      <c r="SO2" s="0"/>
+      <c r="SP2" s="0"/>
+      <c r="SQ2" s="0"/>
+      <c r="SR2" s="0"/>
+      <c r="SS2" s="0"/>
+      <c r="ST2" s="0"/>
+      <c r="SU2" s="0"/>
+      <c r="SV2" s="0"/>
+      <c r="SW2" s="0"/>
+      <c r="SX2" s="0"/>
+      <c r="SY2" s="0"/>
+      <c r="SZ2" s="0"/>
+      <c r="TA2" s="0"/>
+      <c r="TB2" s="0"/>
+      <c r="TC2" s="0"/>
+      <c r="TD2" s="0"/>
+      <c r="TE2" s="0"/>
+      <c r="TF2" s="0"/>
+      <c r="TG2" s="0"/>
+      <c r="TH2" s="0"/>
+      <c r="TI2" s="0"/>
+      <c r="TJ2" s="0"/>
+      <c r="TK2" s="0"/>
+      <c r="TL2" s="0"/>
+      <c r="TM2" s="0"/>
+      <c r="TN2" s="0"/>
+      <c r="TO2" s="0"/>
+      <c r="TP2" s="0"/>
+      <c r="TQ2" s="0"/>
+      <c r="TR2" s="0"/>
+      <c r="TS2" s="0"/>
+      <c r="TT2" s="0"/>
+      <c r="TU2" s="0"/>
+      <c r="TV2" s="0"/>
+      <c r="TW2" s="0"/>
+      <c r="TX2" s="0"/>
+      <c r="TY2" s="0"/>
+      <c r="TZ2" s="0"/>
+      <c r="UA2" s="0"/>
+      <c r="UB2" s="0"/>
+      <c r="UC2" s="0"/>
+      <c r="UD2" s="0"/>
+      <c r="UE2" s="0"/>
+      <c r="UF2" s="0"/>
+      <c r="UG2" s="0"/>
+      <c r="UH2" s="0"/>
+      <c r="UI2" s="0"/>
+      <c r="UJ2" s="0"/>
+      <c r="UK2" s="0"/>
+      <c r="UL2" s="0"/>
+      <c r="UM2" s="0"/>
+      <c r="UN2" s="0"/>
+      <c r="UO2" s="0"/>
+      <c r="UP2" s="0"/>
+      <c r="UQ2" s="0"/>
+      <c r="UR2" s="0"/>
+      <c r="US2" s="0"/>
+      <c r="UT2" s="0"/>
+      <c r="UU2" s="0"/>
+      <c r="UV2" s="0"/>
+      <c r="UW2" s="0"/>
+      <c r="UX2" s="0"/>
+      <c r="UY2" s="0"/>
+      <c r="UZ2" s="0"/>
+      <c r="VA2" s="0"/>
+      <c r="VB2" s="0"/>
+      <c r="VC2" s="0"/>
+      <c r="VD2" s="0"/>
+      <c r="VE2" s="0"/>
+      <c r="VF2" s="0"/>
+      <c r="VG2" s="0"/>
+      <c r="VH2" s="0"/>
+      <c r="VI2" s="0"/>
+      <c r="VJ2" s="0"/>
+      <c r="VK2" s="0"/>
+      <c r="VL2" s="0"/>
+      <c r="VM2" s="0"/>
+      <c r="VN2" s="0"/>
+      <c r="VO2" s="0"/>
+      <c r="VP2" s="0"/>
+      <c r="VQ2" s="0"/>
+      <c r="VR2" s="0"/>
+      <c r="VS2" s="0"/>
+      <c r="VT2" s="0"/>
+      <c r="VU2" s="0"/>
+      <c r="VV2" s="0"/>
+      <c r="VW2" s="0"/>
+      <c r="VX2" s="0"/>
+      <c r="VY2" s="0"/>
+      <c r="VZ2" s="0"/>
+      <c r="WA2" s="0"/>
+      <c r="WB2" s="0"/>
+      <c r="WC2" s="0"/>
+      <c r="WD2" s="0"/>
+      <c r="WE2" s="0"/>
+      <c r="WF2" s="0"/>
+      <c r="WG2" s="0"/>
+      <c r="WH2" s="0"/>
+      <c r="WI2" s="0"/>
+      <c r="WJ2" s="0"/>
+      <c r="WK2" s="0"/>
+      <c r="WL2" s="0"/>
+      <c r="WM2" s="0"/>
+      <c r="WN2" s="0"/>
+      <c r="WO2" s="0"/>
+      <c r="WP2" s="0"/>
+      <c r="WQ2" s="0"/>
+      <c r="WR2" s="0"/>
+      <c r="WS2" s="0"/>
+      <c r="WT2" s="0"/>
+      <c r="WU2" s="0"/>
+      <c r="WV2" s="0"/>
+      <c r="WW2" s="0"/>
+      <c r="WX2" s="0"/>
+      <c r="WY2" s="0"/>
+      <c r="WZ2" s="0"/>
+      <c r="XA2" s="0"/>
+      <c r="XB2" s="0"/>
+      <c r="XC2" s="0"/>
+      <c r="XD2" s="0"/>
+      <c r="XE2" s="0"/>
+      <c r="XF2" s="0"/>
+      <c r="XG2" s="0"/>
+      <c r="XH2" s="0"/>
+      <c r="XI2" s="0"/>
+      <c r="XJ2" s="0"/>
+      <c r="XK2" s="0"/>
+      <c r="XL2" s="0"/>
+      <c r="XM2" s="0"/>
+      <c r="XN2" s="0"/>
+      <c r="XO2" s="0"/>
+      <c r="XP2" s="0"/>
+      <c r="XQ2" s="0"/>
+      <c r="XR2" s="0"/>
+      <c r="XS2" s="0"/>
+      <c r="XT2" s="0"/>
+      <c r="XU2" s="0"/>
+      <c r="XV2" s="0"/>
+      <c r="XW2" s="0"/>
+      <c r="XX2" s="0"/>
+      <c r="XY2" s="0"/>
+      <c r="XZ2" s="0"/>
+      <c r="YA2" s="0"/>
+      <c r="YB2" s="0"/>
+      <c r="YC2" s="0"/>
+      <c r="YD2" s="0"/>
+      <c r="YE2" s="0"/>
+      <c r="YF2" s="0"/>
+      <c r="YG2" s="0"/>
+      <c r="YH2" s="0"/>
+      <c r="YI2" s="0"/>
+      <c r="YJ2" s="0"/>
+      <c r="YK2" s="0"/>
+      <c r="YL2" s="0"/>
+      <c r="YM2" s="0"/>
+      <c r="YN2" s="0"/>
+      <c r="YO2" s="0"/>
+      <c r="YP2" s="0"/>
+      <c r="YQ2" s="0"/>
+      <c r="YR2" s="0"/>
+      <c r="YS2" s="0"/>
+      <c r="YT2" s="0"/>
+      <c r="YU2" s="0"/>
+      <c r="YV2" s="0"/>
+      <c r="YW2" s="0"/>
+      <c r="YX2" s="0"/>
+      <c r="YY2" s="0"/>
+      <c r="YZ2" s="0"/>
+      <c r="ZA2" s="0"/>
+      <c r="ZB2" s="0"/>
+      <c r="ZC2" s="0"/>
+      <c r="ZD2" s="0"/>
+      <c r="ZE2" s="0"/>
+      <c r="ZF2" s="0"/>
+      <c r="ZG2" s="0"/>
+      <c r="ZH2" s="0"/>
+      <c r="ZI2" s="0"/>
+      <c r="ZJ2" s="0"/>
+      <c r="ZK2" s="0"/>
+      <c r="ZL2" s="0"/>
+      <c r="ZM2" s="0"/>
+      <c r="ZN2" s="0"/>
+      <c r="ZO2" s="0"/>
+      <c r="ZP2" s="0"/>
+      <c r="ZQ2" s="0"/>
+      <c r="ZR2" s="0"/>
+      <c r="ZS2" s="0"/>
+      <c r="ZT2" s="0"/>
+      <c r="ZU2" s="0"/>
+      <c r="ZV2" s="0"/>
+      <c r="ZW2" s="0"/>
+      <c r="ZX2" s="0"/>
+      <c r="ZY2" s="0"/>
+      <c r="ZZ2" s="0"/>
+      <c r="AAA2" s="0"/>
+      <c r="AAB2" s="0"/>
+      <c r="AAC2" s="0"/>
+      <c r="AAD2" s="0"/>
+      <c r="AAE2" s="0"/>
+      <c r="AAF2" s="0"/>
+      <c r="AAG2" s="0"/>
+      <c r="AAH2" s="0"/>
+      <c r="AAI2" s="0"/>
+      <c r="AAJ2" s="0"/>
+      <c r="AAK2" s="0"/>
+      <c r="AAL2" s="0"/>
+      <c r="AAM2" s="0"/>
+      <c r="AAN2" s="0"/>
+      <c r="AAO2" s="0"/>
+      <c r="AAP2" s="0"/>
+      <c r="AAQ2" s="0"/>
+      <c r="AAR2" s="0"/>
+      <c r="AAS2" s="0"/>
+      <c r="AAT2" s="0"/>
+      <c r="AAU2" s="0"/>
+      <c r="AAV2" s="0"/>
+      <c r="AAW2" s="0"/>
+      <c r="AAX2" s="0"/>
+      <c r="AAY2" s="0"/>
+      <c r="AAZ2" s="0"/>
+      <c r="ABA2" s="0"/>
+      <c r="ABB2" s="0"/>
+      <c r="ABC2" s="0"/>
+      <c r="ABD2" s="0"/>
+      <c r="ABE2" s="0"/>
+      <c r="ABF2" s="0"/>
+      <c r="ABG2" s="0"/>
+      <c r="ABH2" s="0"/>
+      <c r="ABI2" s="0"/>
+      <c r="ABJ2" s="0"/>
+      <c r="ABK2" s="0"/>
+      <c r="ABL2" s="0"/>
+      <c r="ABM2" s="0"/>
+      <c r="ABN2" s="0"/>
+      <c r="ABO2" s="0"/>
+      <c r="ABP2" s="0"/>
+      <c r="ABQ2" s="0"/>
+      <c r="ABR2" s="0"/>
+      <c r="ABS2" s="0"/>
+      <c r="ABT2" s="0"/>
+      <c r="ABU2" s="0"/>
+      <c r="ABV2" s="0"/>
+      <c r="ABW2" s="0"/>
+      <c r="ABX2" s="0"/>
+      <c r="ABY2" s="0"/>
+      <c r="ABZ2" s="0"/>
+      <c r="ACA2" s="0"/>
+      <c r="ACB2" s="0"/>
+      <c r="ACC2" s="0"/>
+      <c r="ACD2" s="0"/>
+      <c r="ACE2" s="0"/>
+      <c r="ACF2" s="0"/>
+      <c r="ACG2" s="0"/>
+      <c r="ACH2" s="0"/>
+      <c r="ACI2" s="0"/>
+      <c r="ACJ2" s="0"/>
+      <c r="ACK2" s="0"/>
+      <c r="ACL2" s="0"/>
+      <c r="ACM2" s="0"/>
+      <c r="ACN2" s="0"/>
+      <c r="ACO2" s="0"/>
+      <c r="ACP2" s="0"/>
+      <c r="ACQ2" s="0"/>
+      <c r="ACR2" s="0"/>
+      <c r="ACS2" s="0"/>
+      <c r="ACT2" s="0"/>
+      <c r="ACU2" s="0"/>
+      <c r="ACV2" s="0"/>
+      <c r="ACW2" s="0"/>
+      <c r="ACX2" s="0"/>
+      <c r="ACY2" s="0"/>
+      <c r="ACZ2" s="0"/>
+      <c r="ADA2" s="0"/>
+      <c r="ADB2" s="0"/>
+      <c r="ADC2" s="0"/>
+      <c r="ADD2" s="0"/>
+      <c r="ADE2" s="0"/>
+      <c r="ADF2" s="0"/>
+      <c r="ADG2" s="0"/>
+      <c r="ADH2" s="0"/>
+      <c r="ADI2" s="0"/>
+      <c r="ADJ2" s="0"/>
+      <c r="ADK2" s="0"/>
+      <c r="ADL2" s="0"/>
+      <c r="ADM2" s="0"/>
+      <c r="ADN2" s="0"/>
+      <c r="ADO2" s="0"/>
+      <c r="ADP2" s="0"/>
+      <c r="ADQ2" s="0"/>
+      <c r="ADR2" s="0"/>
+      <c r="ADS2" s="0"/>
+      <c r="ADT2" s="0"/>
+      <c r="ADU2" s="0"/>
+      <c r="ADV2" s="0"/>
+      <c r="ADW2" s="0"/>
+      <c r="ADX2" s="0"/>
+      <c r="ADY2" s="0"/>
+      <c r="ADZ2" s="0"/>
+      <c r="AEA2" s="0"/>
+      <c r="AEB2" s="0"/>
+      <c r="AEC2" s="0"/>
+      <c r="AED2" s="0"/>
+      <c r="AEE2" s="0"/>
+      <c r="AEF2" s="0"/>
+      <c r="AEG2" s="0"/>
+      <c r="AEH2" s="0"/>
+      <c r="AEI2" s="0"/>
+      <c r="AEJ2" s="0"/>
+      <c r="AEK2" s="0"/>
+      <c r="AEL2" s="0"/>
+      <c r="AEM2" s="0"/>
+      <c r="AEN2" s="0"/>
+      <c r="AEO2" s="0"/>
+      <c r="AEP2" s="0"/>
+      <c r="AEQ2" s="0"/>
+      <c r="AER2" s="0"/>
+      <c r="AES2" s="0"/>
+      <c r="AET2" s="0"/>
+      <c r="AEU2" s="0"/>
+      <c r="AEV2" s="0"/>
+      <c r="AEW2" s="0"/>
+      <c r="AEX2" s="0"/>
+      <c r="AEY2" s="0"/>
+      <c r="AEZ2" s="0"/>
+      <c r="AFA2" s="0"/>
+      <c r="AFB2" s="0"/>
+      <c r="AFC2" s="0"/>
+      <c r="AFD2" s="0"/>
+      <c r="AFE2" s="0"/>
+      <c r="AFF2" s="0"/>
+      <c r="AFG2" s="0"/>
+      <c r="AFH2" s="0"/>
+      <c r="AFI2" s="0"/>
+      <c r="AFJ2" s="0"/>
+      <c r="AFK2" s="0"/>
+      <c r="AFL2" s="0"/>
+      <c r="AFM2" s="0"/>
+      <c r="AFN2" s="0"/>
+      <c r="AFO2" s="0"/>
+      <c r="AFP2" s="0"/>
+      <c r="AFQ2" s="0"/>
+      <c r="AFR2" s="0"/>
+      <c r="AFS2" s="0"/>
+      <c r="AFT2" s="0"/>
+      <c r="AFU2" s="0"/>
+      <c r="AFV2" s="0"/>
+      <c r="AFW2" s="0"/>
+      <c r="AFX2" s="0"/>
+      <c r="AFY2" s="0"/>
+      <c r="AFZ2" s="0"/>
+      <c r="AGA2" s="0"/>
+      <c r="AGB2" s="0"/>
+      <c r="AGC2" s="0"/>
+      <c r="AGD2" s="0"/>
+      <c r="AGE2" s="0"/>
+      <c r="AGF2" s="0"/>
+      <c r="AGG2" s="0"/>
+      <c r="AGH2" s="0"/>
+      <c r="AGI2" s="0"/>
+      <c r="AGJ2" s="0"/>
+      <c r="AGK2" s="0"/>
+      <c r="AGL2" s="0"/>
+      <c r="AGM2" s="0"/>
+      <c r="AGN2" s="0"/>
+      <c r="AGO2" s="0"/>
+      <c r="AGP2" s="0"/>
+      <c r="AGQ2" s="0"/>
+      <c r="AGR2" s="0"/>
+      <c r="AGS2" s="0"/>
+      <c r="AGT2" s="0"/>
+      <c r="AGU2" s="0"/>
+      <c r="AGV2" s="0"/>
+      <c r="AGW2" s="0"/>
+      <c r="AGX2" s="0"/>
+      <c r="AGY2" s="0"/>
+      <c r="AGZ2" s="0"/>
+      <c r="AHA2" s="0"/>
+      <c r="AHB2" s="0"/>
+      <c r="AHC2" s="0"/>
+      <c r="AHD2" s="0"/>
+      <c r="AHE2" s="0"/>
+      <c r="AHF2" s="0"/>
+      <c r="AHG2" s="0"/>
+      <c r="AHH2" s="0"/>
+      <c r="AHI2" s="0"/>
+      <c r="AHJ2" s="0"/>
+      <c r="AHK2" s="0"/>
+      <c r="AHL2" s="0"/>
+      <c r="AHM2" s="0"/>
+      <c r="AHN2" s="0"/>
+      <c r="AHO2" s="0"/>
+      <c r="AHP2" s="0"/>
+      <c r="AHQ2" s="0"/>
+      <c r="AHR2" s="0"/>
+      <c r="AHS2" s="0"/>
+      <c r="AHT2" s="0"/>
+      <c r="AHU2" s="0"/>
+      <c r="AHV2" s="0"/>
+      <c r="AHW2" s="0"/>
+      <c r="AHX2" s="0"/>
+      <c r="AHY2" s="0"/>
+      <c r="AHZ2" s="0"/>
+      <c r="AIA2" s="0"/>
+      <c r="AIB2" s="0"/>
+      <c r="AIC2" s="0"/>
+      <c r="AID2" s="0"/>
+      <c r="AIE2" s="0"/>
+      <c r="AIF2" s="0"/>
+      <c r="AIG2" s="0"/>
+      <c r="AIH2" s="0"/>
+      <c r="AII2" s="0"/>
+      <c r="AIJ2" s="0"/>
+      <c r="AIK2" s="0"/>
+      <c r="AIL2" s="0"/>
+      <c r="AIM2" s="0"/>
+      <c r="AIN2" s="0"/>
+      <c r="AIO2" s="0"/>
+      <c r="AIP2" s="0"/>
+      <c r="AIQ2" s="0"/>
+      <c r="AIR2" s="0"/>
+      <c r="AIS2" s="0"/>
+      <c r="AIT2" s="0"/>
+      <c r="AIU2" s="0"/>
+      <c r="AIV2" s="0"/>
+      <c r="AIW2" s="0"/>
+      <c r="AIX2" s="0"/>
+      <c r="AIY2" s="0"/>
+      <c r="AIZ2" s="0"/>
+      <c r="AJA2" s="0"/>
+      <c r="AJB2" s="0"/>
+      <c r="AJC2" s="0"/>
+      <c r="AJD2" s="0"/>
+      <c r="AJE2" s="0"/>
+      <c r="AJF2" s="0"/>
+      <c r="AJG2" s="0"/>
+      <c r="AJH2" s="0"/>
+      <c r="AJI2" s="0"/>
+      <c r="AJJ2" s="0"/>
+      <c r="AJK2" s="0"/>
+      <c r="AJL2" s="0"/>
+      <c r="AJM2" s="0"/>
+      <c r="AJN2" s="0"/>
+      <c r="AJO2" s="0"/>
+      <c r="AJP2" s="0"/>
+      <c r="AJQ2" s="0"/>
+      <c r="AJR2" s="0"/>
+      <c r="AJS2" s="0"/>
+      <c r="AJT2" s="0"/>
+      <c r="AJU2" s="0"/>
+      <c r="AJV2" s="0"/>
+      <c r="AJW2" s="0"/>
+      <c r="AJX2" s="0"/>
+      <c r="AJY2" s="0"/>
+      <c r="AJZ2" s="0"/>
+      <c r="AKA2" s="0"/>
+      <c r="AKB2" s="0"/>
+      <c r="AKC2" s="0"/>
+      <c r="AKD2" s="0"/>
+      <c r="AKE2" s="0"/>
+      <c r="AKF2" s="0"/>
+      <c r="AKG2" s="0"/>
+      <c r="AKH2" s="0"/>
+      <c r="AKI2" s="0"/>
+      <c r="AKJ2" s="0"/>
+      <c r="AKK2" s="0"/>
+      <c r="AKL2" s="0"/>
+      <c r="AKM2" s="0"/>
+      <c r="AKN2" s="0"/>
+      <c r="AKO2" s="0"/>
+      <c r="AKP2" s="0"/>
+      <c r="AKQ2" s="0"/>
+      <c r="AKR2" s="0"/>
+      <c r="AKS2" s="0"/>
+      <c r="AKT2" s="0"/>
+      <c r="AKU2" s="0"/>
+      <c r="AKV2" s="0"/>
+      <c r="AKW2" s="0"/>
+      <c r="AKX2" s="0"/>
+      <c r="AKY2" s="0"/>
+      <c r="AKZ2" s="0"/>
+      <c r="ALA2" s="0"/>
+      <c r="ALB2" s="0"/>
+      <c r="ALC2" s="0"/>
+      <c r="ALD2" s="0"/>
+      <c r="ALE2" s="0"/>
+      <c r="ALF2" s="0"/>
+      <c r="ALG2" s="0"/>
+      <c r="ALH2" s="0"/>
+      <c r="ALI2" s="0"/>
+      <c r="ALJ2" s="0"/>
+      <c r="ALK2" s="0"/>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6657,6 +7873,8 @@
       <c r="B4" s="38" t="s">
         <v>315</v>
       </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
       <c r="E4" s="38" t="s">
         <v>316</v>
       </c>
@@ -6674,9 +7892,11 @@
       <c r="D5" s="38" t="s">
         <v>319</v>
       </c>
+      <c r="E5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="39"/>
+      <c r="B6" s="0"/>
       <c r="C6" s="38" t="s">
         <v>320</v>
       </c>
@@ -6689,57 +7909,71 @@
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39"/>
+      <c r="B7" s="0"/>
       <c r="C7" s="38" t="s">
         <v>323</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>324</v>
       </c>
+      <c r="E7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
       <c r="D8" s="38" t="s">
         <v>325</v>
       </c>
+      <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
+      <c r="B9" s="0"/>
       <c r="C9" s="38" t="s">
         <v>326</v>
       </c>
       <c r="D9" s="38" t="s">
         <v>327</v>
       </c>
+      <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
+      <c r="B10" s="0"/>
       <c r="C10" s="38" t="s">
         <v>328</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>329</v>
       </c>
+      <c r="E10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="39"/>
+      <c r="B11" s="0"/>
       <c r="C11" s="38" t="s">
         <v>330</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>331</v>
       </c>
+      <c r="E11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="39"/>
+      <c r="B12" s="0"/>
       <c r="C12" s="38" t="s">
         <v>332</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>333</v>
       </c>
+      <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
+      <c r="B13" s="0"/>
       <c r="C13" s="38" t="s">
         <v>334</v>
       </c>
@@ -6752,12 +7986,14 @@
     </row>
     <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
+      <c r="B14" s="0"/>
       <c r="C14" s="38" t="s">
         <v>337</v>
       </c>
       <c r="D14" s="38" t="s">
         <v>338</v>
       </c>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39" t="n">
@@ -6766,12 +8002,15 @@
       <c r="B15" s="38" t="s">
         <v>339</v>
       </c>
+      <c r="C15" s="0"/>
       <c r="D15" s="38" t="s">
         <v>340</v>
       </c>
+      <c r="E15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
+      <c r="B16" s="0"/>
       <c r="C16" s="38" t="s">
         <v>341</v>
       </c>
@@ -6784,21 +8023,25 @@
     </row>
     <row r="17" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
+      <c r="B17" s="0"/>
       <c r="C17" s="38" t="s">
         <v>344</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>345</v>
       </c>
+      <c r="E17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
+      <c r="B18" s="0"/>
       <c r="C18" s="38" t="s">
         <v>346</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>347</v>
       </c>
+      <c r="E18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="39" t="n">
@@ -6813,27 +8056,33 @@
       <c r="D19" s="38" t="s">
         <v>350</v>
       </c>
+      <c r="E19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
+      <c r="B20" s="0"/>
       <c r="C20" s="38" t="s">
         <v>351</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>352</v>
       </c>
+      <c r="E20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
+      <c r="B21" s="0"/>
       <c r="C21" s="38" t="s">
         <v>353</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>354</v>
       </c>
+      <c r="E21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="39"/>
+      <c r="B22" s="0"/>
       <c r="C22" s="38" t="s">
         <v>355</v>
       </c>
@@ -6859,14 +8108,17 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
       <c r="C24" s="38" t="s">
         <v>362</v>
       </c>
       <c r="D24" s="38" t="s">
         <v>363</v>
       </c>
+      <c r="E24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
       <c r="C25" s="38" t="s">
         <v>364</v>
       </c>
@@ -6878,22 +8130,27 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
       <c r="C26" s="38" t="s">
         <v>367</v>
       </c>
       <c r="D26" s="38" t="s">
         <v>368</v>
       </c>
+      <c r="E26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
       <c r="C27" s="38" t="s">
         <v>369</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>370</v>
       </c>
+      <c r="E27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0"/>
       <c r="C28" s="38" t="s">
         <v>371</v>
       </c>
@@ -6905,46 +8162,57 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="303.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0"/>
       <c r="C29" s="37" t="s">
         <v>374</v>
       </c>
       <c r="D29" s="38" t="s">
         <v>375</v>
       </c>
+      <c r="E29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0"/>
       <c r="C30" s="38" t="s">
         <v>376</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>377</v>
       </c>
+      <c r="E30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0"/>
       <c r="C31" s="38" t="s">
         <v>378</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>379</v>
       </c>
+      <c r="E31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0"/>
       <c r="C32" s="38" t="s">
         <v>380</v>
       </c>
       <c r="D32" s="38" t="s">
         <v>381</v>
       </c>
+      <c r="E32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0"/>
       <c r="C33" s="38" t="s">
         <v>382</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>383</v>
       </c>
+      <c r="E33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0"/>
       <c r="C34" s="38" t="s">
         <v>384</v>
       </c>
@@ -6956,14 +8224,17 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0"/>
       <c r="C35" s="38" t="s">
         <v>387</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>388</v>
       </c>
+      <c r="E35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0"/>
       <c r="C36" s="38" t="s">
         <v>389</v>
       </c>
@@ -6975,6 +8246,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0"/>
       <c r="C37" s="38" t="s">
         <v>392</v>
       </c>
@@ -6995,40 +8267,50 @@
       <c r="D38" s="38" t="s">
         <v>397</v>
       </c>
+      <c r="E38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="415.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0"/>
       <c r="C39" s="38" t="s">
         <v>398</v>
       </c>
       <c r="D39" s="38" t="s">
         <v>399</v>
       </c>
+      <c r="E39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0"/>
       <c r="C40" s="38" t="s">
         <v>400</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>401</v>
       </c>
+      <c r="E40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0"/>
       <c r="C41" s="38" t="s">
         <v>402</v>
       </c>
       <c r="D41" s="38" t="s">
         <v>403</v>
       </c>
+      <c r="E41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0"/>
       <c r="C42" s="38" t="s">
         <v>404</v>
       </c>
       <c r="D42" s="38" t="s">
         <v>405</v>
       </c>
+      <c r="E42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0"/>
       <c r="C43" s="38" t="s">
         <v>406</v>
       </c>
@@ -7049,134 +8331,167 @@
       <c r="D44" s="38" t="s">
         <v>411</v>
       </c>
+      <c r="E44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0"/>
       <c r="C45" s="38" t="s">
         <v>412</v>
       </c>
       <c r="D45" s="38" t="s">
         <v>413</v>
       </c>
+      <c r="E45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0"/>
       <c r="C46" s="38" t="s">
         <v>414</v>
       </c>
       <c r="D46" s="38" t="s">
         <v>415</v>
       </c>
+      <c r="E46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0"/>
       <c r="C47" s="38" t="s">
         <v>416</v>
       </c>
       <c r="D47" s="38" t="s">
         <v>417</v>
       </c>
+      <c r="E47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0"/>
       <c r="C48" s="38" t="s">
         <v>418</v>
       </c>
       <c r="D48" s="38" t="s">
         <v>419</v>
       </c>
+      <c r="E48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0"/>
       <c r="C49" s="38" t="s">
         <v>420</v>
       </c>
       <c r="D49" s="38" t="s">
         <v>421</v>
       </c>
+      <c r="E49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0"/>
       <c r="C50" s="38" t="s">
         <v>422</v>
       </c>
       <c r="D50" s="38" t="s">
         <v>423</v>
       </c>
+      <c r="E50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0"/>
       <c r="C51" s="38" t="s">
         <v>424</v>
       </c>
       <c r="D51" s="38" t="s">
         <v>425</v>
       </c>
+      <c r="E51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="449.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0"/>
       <c r="C52" s="38" t="s">
         <v>426</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>427</v>
       </c>
+      <c r="E52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="415.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0"/>
       <c r="C53" s="38" t="s">
         <v>428</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>429</v>
       </c>
+      <c r="E53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0"/>
       <c r="C54" s="38" t="s">
         <v>430</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>431</v>
       </c>
+      <c r="E54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0"/>
       <c r="C55" s="38" t="s">
         <v>432</v>
       </c>
       <c r="D55" s="38" t="s">
         <v>433</v>
       </c>
+      <c r="E55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0"/>
       <c r="C56" s="38" t="s">
         <v>434</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>435</v>
       </c>
+      <c r="E56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0"/>
       <c r="C57" s="38" t="s">
         <v>436</v>
       </c>
       <c r="D57" s="38" t="s">
         <v>437</v>
       </c>
+      <c r="E57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="426.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0"/>
       <c r="C58" s="38" t="s">
         <v>438</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>439</v>
       </c>
+      <c r="E58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0"/>
       <c r="C59" s="38" t="s">
         <v>440</v>
       </c>
       <c r="D59" s="38" t="s">
         <v>441</v>
       </c>
+      <c r="E59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0"/>
       <c r="C60" s="38" t="s">
         <v>442</v>
       </c>
       <c r="D60" s="38" t="s">
         <v>443</v>
       </c>
+      <c r="E60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="38" t="s">
@@ -7188,24 +8503,30 @@
       <c r="D61" s="38" t="s">
         <v>446</v>
       </c>
+      <c r="E61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0"/>
       <c r="C62" s="38" t="s">
         <v>447</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>448</v>
       </c>
+      <c r="E62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0"/>
       <c r="C63" s="38" t="s">
         <v>449</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>450</v>
       </c>
+      <c r="E63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="438.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0"/>
       <c r="C64" s="38" t="s">
         <v>451</v>
       </c>
@@ -7217,14 +8538,17 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0"/>
       <c r="C65" s="38" t="s">
         <v>454</v>
       </c>
       <c r="D65" s="38" t="s">
         <v>455</v>
       </c>
+      <c r="E65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="258.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0"/>
       <c r="C66" s="38" t="s">
         <v>456</v>
       </c>
@@ -7236,22 +8560,27 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0"/>
       <c r="C67" s="38" t="s">
         <v>459</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>460</v>
       </c>
+      <c r="E67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0"/>
       <c r="C68" s="38" t="s">
         <v>461</v>
       </c>
       <c r="D68" s="38" t="s">
         <v>462</v>
       </c>
+      <c r="E68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0"/>
       <c r="C69" s="38" t="s">
         <v>463</v>
       </c>
@@ -7263,14 +8592,17 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0"/>
       <c r="C70" s="38" t="s">
         <v>466</v>
       </c>
       <c r="D70" s="38" t="s">
         <v>467</v>
       </c>
+      <c r="E70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0"/>
       <c r="C71" s="38" t="s">
         <v>468</v>
       </c>
@@ -7282,22 +8614,27 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0"/>
       <c r="C72" s="38" t="s">
         <v>471</v>
       </c>
       <c r="D72" s="38" t="s">
         <v>472</v>
       </c>
+      <c r="E72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0"/>
       <c r="C73" s="38" t="s">
         <v>473</v>
       </c>
       <c r="D73" s="38" t="s">
         <v>474</v>
       </c>
+      <c r="E73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0"/>
       <c r="C74" s="38" t="s">
         <v>475</v>
       </c>
@@ -7309,6 +8646,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0"/>
       <c r="C75" s="38" t="s">
         <v>478</v>
       </c>
@@ -7320,14 +8658,17 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="303.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0"/>
       <c r="C76" s="38" t="s">
         <v>481</v>
       </c>
       <c r="D76" s="38" t="s">
         <v>482</v>
       </c>
+      <c r="E76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0"/>
       <c r="C77" s="38" t="s">
         <v>483</v>
       </c>
@@ -7348,16 +8689,20 @@
       <c r="D78" s="38" t="s">
         <v>488</v>
       </c>
+      <c r="E78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0"/>
       <c r="C79" s="38" t="s">
         <v>489</v>
       </c>
       <c r="D79" s="37" t="s">
         <v>490</v>
       </c>
+      <c r="E79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0"/>
       <c r="C80" s="38" t="s">
         <v>491</v>
       </c>
@@ -7369,6 +8714,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="0"/>
       <c r="C81" s="38" t="s">
         <v>494</v>
       </c>
@@ -7380,14 +8726,17 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0"/>
       <c r="C82" s="38" t="s">
         <v>497</v>
       </c>
       <c r="D82" s="38" t="s">
         <v>498</v>
       </c>
+      <c r="E82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="0"/>
       <c r="C83" s="38" t="s">
         <v>499</v>
       </c>
@@ -7399,6 +8748,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0"/>
       <c r="C84" s="38" t="s">
         <v>502</v>
       </c>
@@ -7410,6 +8760,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="0"/>
       <c r="C85" s="38" t="s">
         <v>505</v>
       </c>
@@ -7421,30 +8772,37 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="0"/>
       <c r="C86" s="38" t="s">
         <v>508</v>
       </c>
       <c r="D86" s="38" t="s">
         <v>509</v>
       </c>
+      <c r="E86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="0"/>
       <c r="C87" s="38" t="s">
         <v>510</v>
       </c>
       <c r="D87" s="38" t="s">
         <v>511</v>
       </c>
+      <c r="E87" s="0"/>
     </row>
     <row r="88" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="0"/>
       <c r="C88" s="38" t="s">
         <v>512</v>
       </c>
       <c r="D88" s="38" t="s">
         <v>513</v>
       </c>
+      <c r="E88" s="0"/>
     </row>
     <row r="89" customFormat="false" ht="438.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0"/>
       <c r="C89" s="38" t="s">
         <v>514</v>
       </c>
@@ -7456,44 +8814,54 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0"/>
       <c r="C90" s="38" t="s">
         <v>517</v>
       </c>
       <c r="D90" s="38" t="s">
         <v>518</v>
       </c>
+      <c r="E90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0"/>
       <c r="C91" s="38" t="s">
         <v>519</v>
       </c>
       <c r="D91" s="38" t="s">
         <v>520</v>
       </c>
+      <c r="E91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0"/>
       <c r="C92" s="38" t="s">
         <v>521</v>
       </c>
       <c r="D92" s="38" t="s">
         <v>522</v>
       </c>
+      <c r="E92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0"/>
       <c r="C93" s="38" t="s">
         <v>523</v>
       </c>
       <c r="D93" s="38" t="s">
         <v>524</v>
       </c>
+      <c r="E93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0"/>
       <c r="C94" s="38" t="s">
         <v>525</v>
       </c>
       <c r="D94" s="38" t="s">
         <v>526</v>
       </c>
+      <c r="E94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="38" t="s">
@@ -7505,32 +8873,40 @@
       <c r="D95" s="38" t="s">
         <v>529</v>
       </c>
+      <c r="E95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="0"/>
       <c r="C96" s="38" t="s">
         <v>530</v>
       </c>
       <c r="D96" s="38" t="s">
         <v>531</v>
       </c>
+      <c r="E96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="0"/>
       <c r="C97" s="38" t="s">
         <v>532</v>
       </c>
       <c r="D97" s="38" t="s">
         <v>533</v>
       </c>
+      <c r="E97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0"/>
       <c r="C98" s="38" t="s">
         <v>534</v>
       </c>
       <c r="D98" s="38" t="s">
         <v>535</v>
       </c>
+      <c r="E98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0"/>
       <c r="C99" s="38" t="s">
         <v>536</v>
       </c>
@@ -7542,30 +8918,37 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0"/>
       <c r="C100" s="38" t="s">
         <v>539</v>
       </c>
       <c r="D100" s="38" t="s">
         <v>540</v>
       </c>
+      <c r="E100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0"/>
       <c r="C101" s="38" t="s">
         <v>541</v>
       </c>
       <c r="D101" s="38" t="s">
         <v>542</v>
       </c>
+      <c r="E101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="0"/>
       <c r="C102" s="38" t="s">
         <v>543</v>
       </c>
       <c r="D102" s="38" t="s">
         <v>544</v>
       </c>
+      <c r="E102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0"/>
       <c r="C103" s="38" t="s">
         <v>545</v>
       </c>
@@ -7577,70 +8960,87 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="438.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="0"/>
       <c r="C104" s="38" t="s">
         <v>548</v>
       </c>
       <c r="D104" s="38" t="s">
         <v>549</v>
       </c>
+      <c r="E104" s="0"/>
     </row>
     <row r="105" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="0"/>
       <c r="C105" s="38" t="s">
         <v>550</v>
       </c>
       <c r="D105" s="38" t="s">
         <v>551</v>
       </c>
+      <c r="E105" s="0"/>
     </row>
     <row r="106" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="0"/>
       <c r="C106" s="38" t="s">
         <v>552</v>
       </c>
       <c r="D106" s="38" t="s">
         <v>553</v>
       </c>
+      <c r="E106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="0"/>
       <c r="C107" s="38" t="s">
         <v>554</v>
       </c>
       <c r="D107" s="38" t="s">
         <v>555</v>
       </c>
+      <c r="E107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="0"/>
       <c r="C108" s="38" t="s">
         <v>556</v>
       </c>
       <c r="D108" s="38" t="s">
         <v>557</v>
       </c>
+      <c r="E108" s="0"/>
     </row>
     <row r="109" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="0"/>
       <c r="C109" s="38" t="s">
         <v>558</v>
       </c>
       <c r="D109" s="38" t="s">
         <v>559</v>
       </c>
+      <c r="E109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="0"/>
       <c r="C110" s="38" t="s">
         <v>560</v>
       </c>
       <c r="D110" s="37" t="s">
         <v>561</v>
       </c>
+      <c r="E110" s="0"/>
     </row>
     <row r="111" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0"/>
       <c r="C111" s="38" t="s">
         <v>562</v>
       </c>
       <c r="D111" s="37" t="s">
         <v>563</v>
       </c>
+      <c r="E111" s="0"/>
     </row>
     <row r="112" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0"/>
       <c r="C112" s="38" t="s">
         <v>564</v>
       </c>
@@ -7661,24 +9061,30 @@
       <c r="D113" s="38" t="s">
         <v>569</v>
       </c>
+      <c r="E113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="303.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0"/>
       <c r="C114" s="38" t="s">
         <v>570</v>
       </c>
       <c r="D114" s="38" t="s">
         <v>571</v>
       </c>
+      <c r="E114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0"/>
       <c r="C115" s="38" t="s">
         <v>572</v>
       </c>
       <c r="D115" s="38" t="s">
         <v>573</v>
       </c>
+      <c r="E115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="0"/>
       <c r="C116" s="38" t="s">
         <v>574</v>
       </c>
@@ -7690,14 +9096,17 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0"/>
       <c r="C117" s="38" t="s">
         <v>577</v>
       </c>
       <c r="D117" s="38" t="s">
         <v>578</v>
       </c>
+      <c r="E117" s="0"/>
     </row>
     <row r="118" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0"/>
       <c r="C118" s="38" t="s">
         <v>579</v>
       </c>
@@ -7709,46 +9118,57 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0"/>
       <c r="C119" s="38" t="s">
         <v>582</v>
       </c>
       <c r="D119" s="38" t="s">
         <v>583</v>
       </c>
+      <c r="E119" s="0"/>
     </row>
     <row r="120" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="0"/>
       <c r="C120" s="38" t="s">
         <v>584</v>
       </c>
       <c r="D120" s="38" t="s">
         <v>585</v>
       </c>
+      <c r="E120" s="0"/>
     </row>
     <row r="121" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="0"/>
       <c r="C121" s="38" t="s">
         <v>586</v>
       </c>
       <c r="D121" s="38" t="s">
         <v>587</v>
       </c>
+      <c r="E121" s="0"/>
     </row>
     <row r="122" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="0"/>
       <c r="C122" s="38" t="s">
         <v>588</v>
       </c>
       <c r="D122" s="38" t="s">
         <v>589</v>
       </c>
+      <c r="E122" s="0"/>
     </row>
     <row r="123" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="0"/>
       <c r="C123" s="38" t="s">
         <v>570</v>
       </c>
       <c r="D123" s="38" t="s">
         <v>590</v>
       </c>
+      <c r="E123" s="0"/>
     </row>
     <row r="124" customFormat="false" ht="426.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="0"/>
       <c r="C124" s="38" t="s">
         <v>591</v>
       </c>
@@ -7769,8 +9189,10 @@
       <c r="D125" s="38" t="s">
         <v>596</v>
       </c>
+      <c r="E125" s="0"/>
     </row>
     <row r="126" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="0"/>
       <c r="C126" s="38" t="s">
         <v>597</v>
       </c>
@@ -7782,12 +9204,18 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="0"/>
       <c r="C127" s="40" t="s">
         <v>600</v>
       </c>
+      <c r="D127" s="0"/>
+      <c r="E127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="0"/>
+      <c r="C128" s="0"/>
       <c r="D128" s="37"/>
+      <c r="E128" s="0"/>
     </row>
     <row r="129" customFormat="false" ht="438.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="38" t="s">
@@ -7799,6 +9227,7 @@
       <c r="D129" s="37" t="s">
         <v>603</v>
       </c>
+      <c r="E129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="38" t="s">
@@ -7807,11 +9236,14 @@
       <c r="D130" s="37" t="s">
         <v>605</v>
       </c>
+      <c r="E130" s="0"/>
     </row>
     <row r="131" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="0"/>
       <c r="D131" s="38" t="s">
         <v>606</v>
       </c>
+      <c r="E131" s="0"/>
     </row>
     <row r="132" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="38" t="s">
@@ -7853,7 +9285,7 @@
       <c r="D135" s="38" t="s">
         <v>617</v>
       </c>
-      <c r="E135" s="41" t="s">
+      <c r="E135" s="37" t="s">
         <v>618</v>
       </c>
     </row>
@@ -7864,6 +9296,7 @@
       <c r="D136" s="38" t="s">
         <v>620</v>
       </c>
+      <c r="E136" s="0"/>
     </row>
     <row r="137" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="38" t="s">
@@ -7872,6 +9305,7 @@
       <c r="D137" s="38" t="s">
         <v>622</v>
       </c>
+      <c r="E137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="38" t="s">
@@ -7880,6 +9314,7 @@
       <c r="D138" s="38" t="s">
         <v>624</v>
       </c>
+      <c r="E138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="38" t="s">
@@ -7932,17 +9367,120 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="41" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="38" width="26.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="79.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="38" width="59.0459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="38" width="25.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="38" width="8.72959183673469"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>633</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>634</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="38" t="s">
+        <v>636</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="38" t="s">
+        <v>638</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="38" t="s">
+        <v>640</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>643</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="38" t="s">
+        <v>645</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>646</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="38" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="38" t="s">
+        <v>649</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>650</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
ldd:: Advanced Char Driver Operations
</commit_message>
<xml_diff>
--- a/short_notes.xlsx
+++ b/short_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="interview preparation" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="727">
   <si>
     <t>Sr No</t>
   </si>
@@ -4381,8 +4381,7 @@
     <t>Creating your /proc file</t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 • Once you have a read_proc function defined, you need to connect it to an entry in the /proc hierarchy. This is done with a call to create_proc_read_entry:
 • Here is the call used by scull to make its /proc function available as /proc/scullmem:
     create_proc_read_entry("scullmem", 0 /* default mode */,NULL /* parent dir */, scull_read_procmem, NULL /* client data */);
@@ -4390,7 +4389,6 @@
 • Entries in /proc, of course, should be removed when the module is unloaded. remove_proc_entry is the function that undoes what create_proc_read_entry already did:
     remove_proc_entry("scullmem", NULL /* parent dir */);
 </t>
-    </r>
   </si>
   <si>
     <t>The seq_file interface</t>
@@ -4478,6 +4476,482 @@
 • There are times when ioctl is the best way to get information, because it runs faster than reading /proc. If some work must be performed on the data before it’s written to the screen, retrieving the data in binary form is more efficient than reading a text file. In addition, ioctl doesn’t require splitting data into fragments smaller than a page.
 • Another interesting advantage of the ioctl approach is that information-retrieval commands can be left in the driver even when debugging would otherwise be disabled. Unlike a /proc file, which is visible to anyone who looks in the directory.
 </t>
+  </si>
+  <si>
+    <t>Advanced Char Driver Operations</t>
+  </si>
+  <si>
+    <t>ioctl</t>
+  </si>
+  <si>
+    <t>
+• The ioctl driver method has a prototype that differs somewhat from the user-space version:
+    int (*ioctl) (struct inode *inode, struct file *filp, unsigned int cmd, unsigned long arg);
+    - The inode and filp pointers are the values corresponding to the file descriptor fd passed on by the application and are the same parameters passed to the open method.
+    - The cmd argument is passed from the user unchanged
+    - the optional arg argument is passed in the form of an unsigned long , regardless of whether it was given by the user as an integer or a pointer.
+    - If the invoking program doesn’t pass a third argument, the arg value received by the driver operation is undefined.
+</t>
+  </si>
+  <si>
+    <t>Choosing the ioctl Commands</t>
+  </si>
+  <si>
+    <t>
+• The ioctl command numbers should be unique across the system in order to prevent errors caused by issuing the right command to the wrong device.
+• If each ioctl number is unique, the application gets an EINVAL error rather than succeeding in doing something unintended
+• To help programmers create unique ioctl command codes, these codes have been split up into several bitfields.
+• To choose ioctl numbers for your driver according to the Linux kernel convention, you should first check include/asm/ioctl.h and Documentation/ioctl-number.txt.
+• The header defines the bitfields you will be using: type (magic number), ordinal number, direction of transfer, and size of argument.
+• The approved way to define ioctl command numbers uses four bitfields, which have the following meanings. New symbols introduced in this list are defined in &lt;linux/ioctl.h&gt;.
+    - type
+        The magic number. Just choose one number (after consulting ioctl-number.txt) and use it throughout the driver. This field is eight bits wide ( _IOC_TYPEBITS ). 
+    - number 
+        The ordinal (sequential) number. It’s eight bits ( _IOC_NRBITS ) wide. 
+    - direction
+        The direction of data transfer, if the particular command involves a data transfer. The possible values are _IOC_NONE (no data transfer), _IOC_READ , _IOC_WRITE , and _IOC_READ|_IOC_WRITE (data is transferred both ways).
+    - size
+        The size of user data involved. The width of this field is architecture dependent, but is usually 13 or 14 bits. You can find its value for your specific architecture in the macro _IOC_SIZEBITS. It’s not mandatory that you use the size field—the kernel does not check it—but it is a good idea.
+• The header file &lt;asm/ioctl.h&gt;, which is included by &lt;linux/ioctl.h&gt;, defines macros that help set up the command numbers as follows: 
+    _IO(type,nr) (for a command that has no argument), 
+    _IOR(type,nr,datatype) (for reading data from thedriver), 
+    _IOW(type,nr,datatype) (for writing data),
+    _IOWR(type,nr,datatype) (for bidirectional transfers). 
+    The type and number fields are passed as arguments, and the size field is derived by applying sizeof to the datatype argument.
+• The header also defines macros that may be used in your driver to decode the num- bers: _IOC_DIR(nr) , _IOC_TYPE(nr) , _IOC_NR(nr) , and _IOC_SIZE(nr) .
+</t>
+  </si>
+  <si>
+    <t>
+/* Use 'k' as magic number */
+#define SCULL_IOC_MAGIC 'k'
+/* Please use a different 8-bit number in your code */
+#define SCULL_IOCRESET
+_IO(SCULL_IOC_MAGIC, 0)
+/*
+* S means "Set" through a ptr,
+* T means "Tell" directly with the argument value
+* G means "Get": reply by setting through a pointer
+* Q means "Query": response is on the return value
+* X means "eXchange": switch G and S atomically
+* H means "sHift": switch T and Q atomically
+*/
+#define SCULL_IOCSQUANTUM _IOW(SCULL_IOC_MAGIC, 1, int)
+#define SCULL_IOCSQSET _IOW(SCULL_IOC_MAGIC, 2, int)
+#define SCULL_IOCTQUANTUM _IO(SCULL_IOC_MAGIC, 3)
+#define SCULL_IOCTQSET _IO(SCULL_IOC_MAGIC, 4)
+#define SCULL_IOCGQUANTUM _IOR(SCULL_IOC_MAGIC, 5,int)
+#define SCULL_IOCGQSET _IOR(SCULL_IOC_MAGIC, 6,int)
+#define SCULL_IOCQQUANTUM _IO(SCULL_IOC_MAGIC, 7)
+#define SCULL_IOCQQSET _IO(SCULL_IOC_MAGIC, 8)
+#define SCULL_IOCXQUANTUM _IOWR(SCULL_IOC_MAGIC, 9,int)
+#define SCULL_IOCXQSET _IOWR(SCULL_IOC_MAGIC,10,int)
+#define SCULL_IOCHQUANTUM _IO(SCULL_IOC_MAGIC, 11)
+#define SCULL_IOCHQSET _IO(SCULL_IOC_MAGIC, 12)
+#define SCULL_IOC_MAXNR 14
+</t>
+  </si>
+  <si>
+    <t>Predefined command</t>
+  </si>
+  <si>
+    <t>
+• The predefined commands are divided into three groups:
+    • Those that can be issued on any file (regular, device, FIFO, or socket)
+    • Those that are issued only on regular files
+    • Those specific to the filesystem type
+• Device driver writers are interested only in the first group of commands, whose magic number is “T.”
+</t>
+  </si>
+  <si>
+    <t>Using the ioctl Argument</t>
+  </si>
+  <si>
+    <t>
+• If it is an integer, it’s easy: it can be used directly. If it is a pointer, however, some care must be taken.
+• When a pointer is used to refer to user space, we must ensure that the user address is valid. An attempt to access an unverified user-supplied pointer can lead to incorrect behavior, a kernel oops, system corruption, or security problems. It is the driver’s responsibility to make proper checks on every user-space address it uses and to return an error if it is invalid.
+• To start, address verification (without transferring data) is implemented by the function access_ok, which is declared in &lt;asm/uaccess.h&gt;:
+    int access_ok(int type, const void *addr, unsigned long size);
+    - The first argument should be either VERIFY_READ or VERIFY_WRITE , depending on whether the action to be performed is reading the user-space memory area or writing it. 
+    - The addr argument holds a user-space address, and size is a byte count.
+    - access_ok returns a boolean value: 1 for success (access is OK) and 0 for failure (access is not OK). 
+    - If it returns false, the driver should usually return -EFAULT to the caller.
+• the programmer can exploit a set of functions that are optimized for the most used data sizes (one, two, four, and eight bytes). These functions are described in the following list and are defined in &lt;asm/uaccess.h&gt;:
+    put_user(datum, ptr)
+    __put_user(datum, ptr)
+    - These macros write the datum to user space; they are relatively fast and should be called instead of copy_to_user whenever single values are being transferred. The macros have been written to allow the passing of any type of pointer to put_user, as long as it is a user-space address. The size of the data transfer depends on the type of the ptr argument and is determined at compile time using the sizeof and typeof compiler builtins.
+    - put_user checks to ensure that the process is able to write to the given memory address. It returns 0 on success, and -EFAULT on error. 
+    - __put_user performs less checking (it does not call access_ok), but can still fail if the memory pointed to is not writable by the user.
+    - Thus, __put_user should only be used if the memory region has already been verified with access_ok.
+    get_user(local, ptr)
+    __get_user(local, ptr)
+    - These macros are used to retrieve a single datum from user space. They behave like put_user and __put_user, but transfer data in the opposite direction.
+</t>
+  </si>
+  <si>
+    <t>
+int err = 0, tmp;
+int retval = 0;
+/*
+* extract the type and number bitfields, and don't decode
+* wrong cmds: return ENOTTY (inappropriate ioctl) before access_ok( )
+*/
+if (_IOC_TYPE(cmd) != SCULL_IOC_MAGIC) return -ENOTTY;
+if (_IOC_NR(cmd) &gt; SCULL_IOC_MAXNR) return -ENOTTY;
+/*
+* the direction is a bitmask, and VERIFY_WRITE catches R/W
+* transfers. `Type' is user-oriented, while
+* access_ok is kernel-oriented, so the concept of "read" and
+* "write" is reversed
+*/
+if (_IOC_DIR(cmd) &amp; _IOC_READ)
+    err = !access_ok(VERIFY_WRITE, (void __user *)arg, _IOC_SIZE(cmd));
+else if (_IOC_DIR(cmd) &amp; _IOC_WRITE)
+    err = !access_ok(VERIFY_READ, (void __user *)arg, _IOC_SIZE(cmd));
+if (err) return -EFAULT;</t>
+  </si>
+  <si>
+    <t>Capabilities and Restricted Operations</t>
+  </si>
+  <si>
+    <t>
+• a particular user (or program) can be empowered to perform a specific privileged operation without giving away the ability to perform other, unre lated operations. 
+• The kernel uses capabilities exclusively for permissions manage ment and exports two system calls capget and capset, to allow them to be managed from user space. The full set of capabilities can be found in &lt;linux/capability.h&gt;.
+• Before performing a privileged operation, a device driver should check that the calling process has the appropriate capability; failure to do so could result user processes performing unauthorized operations with bad results on system stability or security. 
+• Capability checks are performed with the capable function (defined in &lt;linux/sched.h&gt;):
+    int capable(int capability);
+</t>
+  </si>
+  <si>
+    <t>
+if (! capable (CAP_SYS_ADMIN))
+    return -EPERM;
+</t>
+  </si>
+  <si>
+    <t>Blocking I/O</t>
+  </si>
+  <si>
+    <t>
+• A call to read may come when no data is available, but more is expected in the future. Or a process could attempt to write, but your device is not ready to accept the data, because your output buffer is full. 
+• The calling process usually does not care about such issues; the programmer simply expects to call read or write and have the call return after the necessary work has been done.
+• So, in such cases, your driver should (by default) block the process, putting it to sleep until the request can proceed.
+</t>
+  </si>
+  <si>
+    <r>
+      <t>
+• What does it mean for a process to “sleep”? When a process is put to sleep, it is marked as being in a special state and removed from the scheduler’s run queue. 
+• Until something comes along to change that state, the process will not be scheduled on any CPU and, therefore, will not run. 
+• A sleeping process is waiting for some future event to happen.
+• There are, however, a couple of rules that you must keep in mind to be able to code sleeps in a safe manner.
+    - never sleep when you are running in an atomic context.
+    - You also cannot sleep if you have disabled interrupts. 
+    - It is legal to sleep while holding a semaphore, but you should look very carefully at any code that does so. If code sleeps while holding a semaphore, any other thread waiting for that semaphore also sleeps.
+• Making it possible for your sleeping process to be found is, instead, accomplished through a data structure called a wait queue. A wait queue is just what it sounds like: a list of processes, all waiting for a specific event.
+• a wait queue is managed by means of a “wait queue head,” a structure of type wait_queue_head_t , which is defined in &lt;linux/wait.h&gt;. 
+• A wait queue head can be defined and initialized statically with:
+    DECLARE_WAIT_QUEUE_HEAD(name);
+    or dynamicly as follows:
+    wait_queue_head_t my_queue;
+    init_waitqueue_head(&amp;my_queue);
+    We will return to the structure of wait queues shortly, but we know enough now to take a first look at sleeping and waking up.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>
+• The simplest way of sleeping in the Linux kernel is a macro called wait_event (with a few variants);
+•  it combines handling the details of sleeping with a check on the condition a process is waiting for. The forms of wait_event are:
+    wait_event(queue, condition)
+        wait_event, your process is put into an uninterruptible sleep which is usually not what you want.
+    wait_event_interruptible(queue, condition)
+        The preferred is wait_event_interruptible, which can be interrupted by signals. This version returns an integer value that you should check; a nonzero value means your sleep was interrupted by some sort of signal, and your driver should probably return -ERESTARTSYS .
+    wait_event_timeout(queue, condition, timeout)
+    wait_event_interruptible_timeout(queue, condition, timeout)
+        wait for a limited time; after that time period (expressed in jiffies) expires, the macros return with a value of 0 regardless of how condition evaluates.
+    - In all of the above forms, queue is the wait queue head to use. Notice that it is passed “by value.”
+    - The condition is an arbitrary boolean expression that is evaluated by the macro before and after sleeping; until condition evaluates to a true value, the process continues to sleep. Note that condition may be evaluated an arbitrary number of times, so it should not have any side effects.
+</t>
+  </si>
+  <si>
+    <r>
+      <t>static DECLARE_WAIT_QUEUE_HEAD(wq);
+static int flag = 0;
+ssize_t sleepy_read (struct file *filp, char __user *buf, size_t count, loff_t *pos)
+{
+    printk(KERN_DEBUG "process %i (%s) going to sleep\n", current-&gt;pid, current-&gt;comm);
+    wait_event_interruptible(wq, flag != 0);
+    flag = 0;
+    printk(KERN_DEBUG "awoken %i (%s)\n", current-&gt;pid, current-&gt;comm);
+    return 0; /* EOF */
+}
+ssize_t sleepy_write (struct file *filp, const char __user *buf, size_t count, loff_t *pos)
+{
+    printk(KERN_DEBUG "process %i (%s) awakening the readers...\n", current-&gt;pid, current-&gt;comm);
+    flag = 1;
+    wake_up_interruptible(&amp;wq);
+    return count; /* succeed, to avoid retrial */
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <t>
+• The other half of the picture, of course, is waking up. Some other thread of execution (a different process, or an interrupt handler, perhaps) has to perform the wakeup for you, since your process is, of course, asleep. 
+• The basic function that wakes up sleeping processes is called wake_up. It comes in several forms (but welook at only two of them now):
+    void wake_up(wait_queue_head_t *queue);
+        wake_up wakes up all processes waiting on the given queue. 
+    void wake_up_interruptible(wait_queue_head_t *queue);
+        The other form (wake_up_interruptible) restricts itself to processes performing an interruptible sleep. 
+• In general, the two are indistinguishable (if you are using interruptible sleeps); 
+• in practice, the convention is to use wake_up if you are using wait_event and wake_up_interruptible if you use wait_event_interruptible.
+</t>
+  </si>
+  <si>
+    <t>A Blocking I/O Example</t>
+  </si>
+  <si>
+    <r>
+      <t>
+• an example of a real driver method that implements blocking I/O. This example is taken from the scullpipe driver; it is a special form of scull that implements a pipe-like device.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>how process sleeps</t>
+  </si>
+  <si>
+    <t>
+• The first step in putting a process to sleep is usually the allocation and initialization of a wait_queue_t structure, followed by its addition to the proper wait queue.
+• The next step is to set the state of the process to mark it as being asleep. There are two states that indicate that a process is asleep: TASK_INTERRUPTIBLE and TASK_UNINTERRUPTIBLE
+</t>
+  </si>
+  <si>
+    <t>Manual sleeps</t>
+  </si>
+  <si>
+    <t>
+• The first step is the creation and initialization of a wait queue entry. That is usually done with this macro:
+    DEFINE_WAIT(name);
+        in which name is the name of the wait queue entry variable. You can also do things in two steps:
+        it is usually easier to put a DEFINE_WAIT line at the top of the loop that implements your sleep.
+    wait_queue_t my_wait;
+    init_wait(&amp;my_wait);
+• The next step is to add your wait queue entry to the queue, and set the process state. Both of those tasks are handled by this function:
+    void prepare_to_wait(wait_queue_head_t *queue, wait_queue_t *wait, int state);
+        queue and wait are the wait queue head and the process entry, respectively.
+        state is the new state for the process; it should be either TASK_INTERRUPTIBLE or TASK_UNINTERRUPTIBLE.
+• After calling prepare_to_wait, the process can call schedule()—after it has checked to be sure it still needs to wait. 
+• Once schedule returns, it is cleanup time. That task, too, is handled by a special function:
+    void finish_wait(wait_queue_head_t *queue, wait_queue_t *wait);
+</t>
+  </si>
+  <si>
+    <t>Exclusive waits</t>
+  </si>
+  <si>
+    <t>
+• when a process calls wake_up on a wait queue, all processes waiting on that queue are made runnable. 
+• In many cases, that is the correct behavior. In others, however, it is possible to know ahead of time that only one of the processes being awakened will succeed in obtaining the desired resource, and the rest will simply have to sleep again.
+• The kernel developers added an  “exclusive wait” option to the kernel. An exclusive wait acts very much like a normal sleep, with two important differences:
+    • When a wait queue entry has the WQ_FLAG_EXCLUSIVE flag set, it is added to the end of the wait queue. Entries without that flag are, instead, added to the beginning.
+    • When wake_up is called on a wait queue, it stops after waking the first process that has the WQ_FLAG_EXCLUSIVE flag set.
+• The end result is that processes performing exclusive waits are awakened one at a time, in an orderly manner, and do not create thundering herds. The kernel still wakes up all nonexclusive waiters every time, however.
+• Putting a process into an interruptible wait is a simple matter of calling prepare_to_wait_exclusive:
+    void prepare_to_wait_exclusive(wait_queue_head_t *queue,wait_queue_t *wait,int state);
+        This call, when used in place of prepare_to_wait, sets the “exclusive” flag in the wait queue entry and adds the process to the end of the wait queue.
+</t>
+  </si>
+  <si>
+    <t>The details of waking up</t>
+  </si>
+  <si>
+    <t>
+• wake_up(wait_queue_head_t *queue);
+  wake_up_interruptible(wait_queue_head_t *queue);
+    wake_up awakens every process on the queue that is not in an exclusive wait, and exactly one exclusive waiter, if it exists. wake_up_interruptible does the same, with the exception that it skips over processes in an uninterruptible sleep. These functions can, before returning, cause one or more of the processes awakened to be scheduled.
+• wake_up_nr(wait_queue_head_t *queue, int nr);
+  wake_up_interruptible_nr(wait_queue_head_t *queue, int nr);
+    These functions perform similarly to wake_up, except they can awaken up to nr exclusive waiters, instead of just one. Note that passing 0 is interpreted as asking for all of the exclusive waiters to be awakened, rather than none of them.
+• wake_up_all(wait_queue_head_t *queue);
+  wake_up_interruptible_all(wait_queue_head_t *queue);
+    This form of wake_up awakens all processes whether they are performing an exclusive wait or not (though the interruptible form still skips processes doing uninterruptible waits).
+• wake_up_interruptible_sync(wait_queue_head_t *queue);
+</t>
+  </si>
+  <si>
+    <t>poll and select</t>
+  </si>
+  <si>
+    <t>
+• Applications that use nonblocking I/O often use the poll, select, and epoll system calls as well. poll, select, and epoll have essentially the same functionality: each allow a process to determine whether it can read from or write to one or more open files without blocking.
+• Support for any of these calls requires support from the device driver. This support (for all three calls) is provided through the driver’s poll method. This method has the following prototype:
+    unsigned int (*poll) (struct file *filp, poll_table *wait);
+• The driver method is called whenever the user-space program performs a poll, select, or epoll system call involving a file descriptor associated with the driver. 
+• The device method is in charge of these two steps:
+    1. Call poll_wait on one or more wait queues that could indicate a change in the poll status.If no file descriptors are currently available for I/O, the kernel causes the process to wait on the wait queues for all file descriptors passed to the system call.
+    2. Return a bit mask describing the operations (if any) that could be immediately performed without blocking.
+• The poll_table structure, the second argument to the poll method, is used within the kernel to implement the poll, select, and epoll calls; it is declared in &lt;linux/poll.h&gt;
+• poll_table is passed to the driver method so that the driver can load it with every wait queue that could wake up the process and change the status of the poll operation. The driver adds a wait queue to the poll_table structure by calling the function poll_wait:
+    void poll_wait (struct file *, wait_queue_head_t *, poll_table *);
+• The second task performed by the poll method is returning the bit mask describing which operations could be completed immediately.
+• Several flags (defined via &lt;linux/poll.h&gt;) are used to indicate the possible operations:
+</t>
+  </si>
+  <si>
+    <t>
+POLLIN
+    This bit must be set if the device can be read without blocking.
+POLLRDNORM
+    This bit must be set if “normal” data is available for reading. A readable device returns (POLLIN | POLLRDNORM) .        
+so on ...
+Consider the scullpipe implementation of the poll method:
+static unsigned int scull_p_poll(struct file *filp, poll_table *wait)
+{
+    struct scull_pipe *dev = filp-&gt;private_data;
+    unsigned int mask = 0;
+    /*
+    * The buffer is circular; it is considered full
+    * if "wp" is right behind "rp" and empty if the
+    * two are equal.
+    */
+    down(&amp;dev-&gt;sem);
+    poll_wait(filp, &amp;dev-&gt;inq, wait);
+    poll_wait(filp, &amp;dev-&gt;outq, wait);
+    if (dev-&gt;rp != dev-&gt;wp)
+        mask |= POLLIN | POLLRDNORM;
+    /* readable */
+    if (spacefree(dev))
+        mask |= POLLOUT | POLLWRNORM;
+    /* writable */
+    up(&amp;dev-&gt;sem);
+    return mask;
+}</t>
+  </si>
+  <si>
+    <t>Asynchronous Notification</t>
+  </si>
+  <si>
+    <t>
+• User programs have to execute two steps to enable asynchronous notification from an input file. 
+• First, they specify a process as the “owner” of the file. When a process invokes the F_SETOWN command using the fcntl system call, the process ID of the owner process is saved in filp-&gt;f_owner for later use. This step is necessary for the kernel to know just whom to notify.
+• In order to actually enable asynchronous notification, the user programs must set the FASYNC flag in the device by means of the F_SETFL fcntl command.
+• After these two calls have been executed, the input file can request delivery of a SIGIO signal whenever new data arrives. The signal is sent to the process (or process group, if the value is negative) stored in filp-&gt;f_owner .
+• For example, the following lines of code in a user program enable asynchronous notification to the current process for the stdin input file:
+    signal(SIGIO, &amp;input_handler); /* dummy sample; sigaction( ) is better */
+    fcntl(STDIN_FILENO, F_SETOWN, getpid( ));
+    oflags = fcntl(STDIN_FILENO, F_GETFL);
+    fcntl(STDIN_FILENO, F_SETFL, oflags | FASYNC);
+• however, that not all the devices support asynchronous notification, and you can choose not to offer it. Applications usually assume that the asynchronous capability is available only for sockets and ttys.
+</t>
+  </si>
+  <si>
+    <t>
+Here’s how scullpipe implements the fasync method:
+static int scull_p_fasync(int fd, struct file *filp, int mode)
+{
+    struct scull_pipe *dev = filp-&gt;private_data;
+    return fasync_helper(fd, filp, mode, &amp;dev-&gt;async_queue);
+}
+</t>
+  </si>
+  <si>
+    <t>The llseek Implementation</t>
+  </si>
+  <si>
+    <t>
+• The llseek method implements the lseek and llseek system calls. We have already stated that if the llseek method is missing from the device’s operations, the default implementation in the kernel performs seeks by modifying filp-&gt;f_pos , the current reading/writing position within the file.
+• You may need to provide your own llseek method if the seek operation corresponds to a physical operation on the device. A simple example can be seen in the scull driver:
+• most devices offer a data flow rather than a data area (just think about the serial ports or the keyboard), and seeking those devices does not make sense. If this is the case for your device, you can’t just refrain from declaring the llseek operation, because the default method allows seeking. Instead, you should inform the kernel that your device does not support llseek by calling nonseekable_open in your open method:
+</t>
+  </si>
+  <si>
+    <r>
+      <t>
+loff_t scull_llseek(struct file *filp, loff_t off, int whence) {
+    struct scull_dev *dev = filp-&gt;private_data;
+    loff_t newpos;
+    switch(whence) {
+        case 0: /* SEEK_SET */
+            newpos = off;
+        break;
+        case 1: /* SEEK_CUR */
+            newpos = filp-&gt;f_pos + off;
+        break;
+        case 2: /* SEEK_END */
+            newpos = dev-&gt;size + off;
+        break;
+        default: /* can't happen */
+            return -EINVAL;
+    }
+    if (newpos &lt; 0) return -EINVAL;
+        filp-&gt;f_pos = newpos;
+    return newpos;
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Access Control on a Device File</t>
+  </si>
+  <si>
+    <t>Single-Open Devices</t>
+  </si>
+  <si>
+    <t>• Allowing only a single process to open a device has undesirable properties, but it is also the easiest access control to implement for a device driver, so it’s shown here. The source code is extracted from a device called scullsingle.
+• The scullsingle device maintains an atomic_t variable called scull_s_available ; that variable is initialized to a value of one, indicating that the device is indeed available. The open call decrements and tests scull_s_available and refuses access if somebody else already has the device open:
+</t>
+  </si>
+  <si>
+    <t>
+static atomic_t scull_s_available = ATOMIC_INIT(1);
+static int scull_s_open(struct inode *inode, struct file *filp) {
+    struct scull_dev *dev = &amp;scull_s_device; /* device information */
+    if (! atomic_dec_and_test (&amp;scull_s_available)) {
+        atomic_inc(&amp;scull_s_available);
+        return -EBUSY; /* already open */
+    }
+    /* then, everything else is copied from the bare scull device */
+    if ( (filp-&gt;f_flags &amp; O_ACCMODE) = = O_WRONLY)
+        scull_trim(dev);
+    filp-&gt;private_data = dev;
+    return 0;
+    /* success */
+}
+The release call, on the other hand, marks the device as no longer busy:
+static int scull_s_release(struct inode *inode, struct file *filp) {
+    atomic_inc(&amp;scull_s_available); /* release the device */
+    return 0;
+}</t>
+  </si>
+  <si>
+    <t>Restricting Access to a Single User at a Time</t>
+  </si>
+  <si>
+    <t>
+• The next step beyond a single-open device is to let a single user open a device in multiple processes but allow only one user to have the device open at a time. 
+• This solution makes it easy to test the device, since the user can read and write from several processes at once, but assumes that the user takes some responsibility for maintaining the integrity of the data during multiple accesses.
+• This is accomplished by add ing checks in the open method; such checks are performed after the normal permission checking and can only make access more restrictive than that specified by the owner and group permission bits.
+• The name of the device is sculluid.
+    The open call grants access on first open but remembers the owner of the device.
+    This means that a user can open the device multiple times, thus allowing cooperating processes to work concurrently on the device.
+</t>
+  </si>
+  <si>
+    <t>    spin_lock(&amp;scull_u_lock);
+    if (scull_u_count &amp;&amp;
+        (scull_u_owner != current-&gt;uid) &amp;&amp; /* allow user */
+        (scull_u_owner != current-&gt;euid) &amp;&amp; /* allow whoever did su */
+        !capable(CAP_DAC_OVERRIDE)) { /* still allow root */
+        spin_unlock(&amp;scull_u_lock);
+        return -EBUSY;
+        /* -EPERM would confuse the user */
+    }
+    if (scull_u_count = = 0)
+        scull_u_owner = current-&gt;uid; /* grab it */
+    scull_u_count++;
+    spin_unlock(&amp;scull_u_lock);</t>
   </si>
 </sst>
 </file>
@@ -9671,17 +10145,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="41" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="38" width="26.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="79.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="81.1377551020408"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="38" width="59.0459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="38" width="25.4234693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="38" width="8.72959183673469"/>
@@ -9883,7 +10357,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="37" t="s">
         <v>677</v>
       </c>
     </row>
@@ -9898,6 +10372,187 @@
       </c>
       <c r="D26" s="38" t="s">
         <v>680</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="38" t="s">
+        <v>681</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>682</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="426.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="38" t="s">
+        <v>684</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>685</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="38" t="s">
+        <v>687</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="415.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="38" t="s">
+        <v>689</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>690</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="38" t="s">
+        <v>692</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>693</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="38" t="s">
+        <v>695</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="292.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="38" t="s">
+        <v>695</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="258.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="42" t="s">
+        <v>698</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D35" s="38" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="38" t="s">
+        <v>701</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="38" t="s">
+        <v>703</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="38" t="s">
+        <v>705</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="38" t="s">
+        <v>707</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="38" t="s">
+        <v>709</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="38" t="s">
+        <v>711</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>712</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="38" t="s">
+        <v>714</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>715</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="258.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="38" t="s">
+        <v>717</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>718</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="38" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="38" t="s">
+        <v>721</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>722</v>
+      </c>
+      <c r="E45" s="38" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="38" t="s">
+        <v>724</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>725</v>
+      </c>
+      <c r="E46" s="38" t="s">
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ldd: continue hotplug attribute
</commit_message>
<xml_diff>
--- a/short_notes.xlsx
+++ b/short_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="interview preparation" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="809">
   <si>
     <t>Sr No</t>
   </si>
@@ -6102,6 +6102,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>typedef struct { /* ... */ } wait_queue_head_t;
 void init_waitqueue_head(wait_queue_head_t *queue);
@@ -6114,6 +6115,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>    The defined type for Linux wait queues. A wait_queue_head_t must be explicitly initialized with either init_waitqueue_head at runtime or DECLARE_WAIT_QUEUE_HEAD at compile time.
 </t>
@@ -6125,6 +6127,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>void wait_event(wait_queue_head_t q, int condition);
 int wait_event_interruptible(wait_queue_head_t q, int condition);
@@ -6138,6 +6141,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>    Cause the process to sleep on the given queue until the given condition evaluates to a true value.
 </t>
@@ -7948,6 +7952,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>RQ_NONE, IRQ_HANDLED, IRQ_RETVAL(int x)
  </t>
@@ -7957,6 +7962,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>   The possible return values from an interrupt handler, indicating whether an actual interrupt from the device was present.
 </t>
@@ -7967,6 +7973,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>void disable_irq(int irq);
 void disable_irq_nosync(int irq);
@@ -7978,6 +7985,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>   A driver can enable and disable interrupt reporting. If the hardware tries to generate an interrupt while interrupts are disabled, the interrupt is lost forever. A driver using a shared handler must not use these functions.
 </t>
@@ -7988,6 +7996,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>void local_irq_save(unsigned long flags);
 void local_irq_restore(unsigned long flags);
@@ -7998,6 +8007,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>   Use local_irq_save to disable interrupts on the local processor and remember their previous state. The flags can be passed to local_irq_restore to restore the previous interrupt state.
 </t>
@@ -8008,6 +8018,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>void local_irq_disable(void);
 void local_irq_enable(void);
@@ -8018,10 +8029,297 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>   Functions that unconditionally disable and enable interrupts on the current processor.
 </t>
     </r>
+  </si>
+  <si>
+    <t>Linux Device Model</t>
+  </si>
+  <si>
+    <t>
+• The device model provides that abstraction. It is now used within the kernel to support a wide variety of tasks, including:
+    -  Power management and system shutdown
+    -  Communications with user space
+    -  Hotpluggable devices
+    -  Device classes
+    -  Object lifecycles
+</t>
+  </si>
+  <si>
+    <t>Kobjects basics</t>
+  </si>
+  <si>
+    <t>
+• The kobject is the fundamental structure that holds the device model together.
+• The tasks handled by struct kobject and its supporting code now include:
+    Reference counting of objects
+        tracking the lifecycle of objects is through reference counting. When no code in the kernel holds a reference to a given object, that object has finished its useful life and can be deleted.
+    Sysfs representation
+        Every object that shows up in sysfs has, underneath it, a kobject that interacts with the kernel to create its visible representation.
+    Data structure glue
+        The device model is, in its entirety, a fiendishly complicated data structure made up of multiple hierarchies with numerous links between them.
+    Hotplug event handling
+        The kobject subsystem handles the generation of events that notify user space about the comings and goings of hardware on the system.
+• the way to convert a pointer to a struct kobject called kp embedded within a struct cdev would be:
+    struct cdev *device = container_of(kp, struct cdev, kobj);
+</t>
+  </si>
+  <si>
+    <t>kobject initialization</t>
+  </si>
+  <si>
+    <t>
+• The first of those is to simply set the entire kobject to 0 , usually with a call to memset.
+• The next step is to set up some of the internal fields with a call to kobject_init( ):
+    void kobject_init(struct kobject *kobj);
+    - Among other things, kobject_init sets the kobject’s reference count to one. 
+    - Calling kobject_init is not sufficient, however. Kobject users must, at a minimum, set the name of the kobject; this is the name that is used in sysfs entries.
+    int kobject_set_name(struct kobject *kobj, const char *format, ...);
+    - This function takes a printk-style variable argument list. Believe it or not, it is actually possible for this operation to fail (it may try to allocate memory); 
+    - conscientious code should check the return value and react accordingly.
+• The other kobject fields that should be set, directly or indirectly, by the creator are ktype , kset , and parent .
+</t>
+  </si>
+  <si>
+    <t>Reference count manipulation</t>
+  </si>
+  <si>
+    <t>
+• As long as references to the object exist, the object (and the code that supports it) must continue to exist. 
+• The low-level functions for manipulating a kobject’s reference counts are:
+    struct kobject *kobject_get(struct kobject *kobj);
+    void kobject_put(struct kobject *kobj);
+    - A successful call to kobject_get increments the kobject’s reference counter and returns a pointer to the kobject. 
+    - If, however, the kobject is already in the process of being destroyed, the operation fails, and kobject_get returns NULL . 
+    - This return value must always be tested, or no end of unpleasant race conditions could result.
+    - When a reference is released, the call to kobject_put decrements the reference count and, possibly, frees the object. 
+• Remember that kobject_init sets the reference count to one; so when you create a kobject, you should make sure that the corresponding kobject_put call is made when that initial reference is no longer needed.
+</t>
+  </si>
+  <si>
+    <t>Release functions and kobject types</t>
+  </si>
+  <si>
+    <t>
+• The reference count is not under the direct control of the code that created the kobject. So that code must be notified asynchronously whenever the last reference to one of its kobjects goes away.
+• This notification is done through a kobject’s release method.
+• Interestingly, the release method is not stored in the kobject itself; instead, it is associated with the type of the structure that contains the kobject. 
+• This type is tracked with a structure of type struct kobj_type , often simply called a “ktype.” This structure looks like the following:
+• Every kobject needs to have an associated kobj_type structure. Confusingly, the pointer to this structure can be found in two different places.
+• The kobject structure itself contains a field (called ktype ) that can contain this pointer.
+• the following macro finds the kobj_type pointer for a given kobject:
+    struct kobj_type *get_ktype(struct kobject *kobj);
+</t>
+  </si>
+  <si>
+    <t>struct kobj_type {
+    void (*release)(struct kobject *);
+    struct sysfs_ops *sysfs_ops;
+    struct attribute **default_attrs;
+};</t>
+  </si>
+  <si>
+    <t>Kobject Hierarchies</t>
+  </si>
+  <si>
+    <t>
+• The kobject structure is often used to link together objects into a hierarchical structure that matches the structure of the subsystem being modeled. 
+• There are two separate mechanisms for this linking: the parent pointer and ksets.
+• The parent field in struct kobject is a pointer to another kobject—the one representing the next level up in the hierarchy.
+• The main use for the parent pointer is to position the object in the sysfs hierarchy.
+</t>
+  </si>
+  <si>
+    <t>Ksets</t>
+  </si>
+  <si>
+    <t>
+• a kset looks like an extension of the kobj_type structure; a kset is a collection of kobjects embedded within structures of the same type.
+• It is worth noting that ksets are always represented in sysfs; once a kset has been set up and added to the system, there will be a sysfs directory for it. 
+• Kobjects do not necessarily show up in sysfs, but every kobject that is a member of a kset is represented there.
+• Adding a kobject to a kset is usually done when the object is created; it is a two-step process. 
+• The kobject’s kset field must be pointed at the kset of interest; then the kobject should be passed to:
+    int kobject_add(struct kobject *kobj);
+• function is simply a combination of kobject_init and kobject_add.
+    extern int kobject_register(struct kobject *kobj);
+• At some point, the kobject will probably have to be removed from the kset to clear that reference; that is done with:
+    void kobject_del(struct kobject *kobj);
+• There is also a kobject_unregister function, which is a combination of kobject_del and kobject_put.
+• A kset keeps its children in a standard kernel linked list. In almost all cases, the contained kobjects also have pointers to the kset (or, strictly, its embedded kobject) in their parent’s fields.
+</t>
+  </si>
+  <si>
+    <t>Operations on ksets</t>
+  </si>
+  <si>
+    <t>
+• For initialization and setup, ksets have an interface very similar to that of kobjects.
+• The following functions exist:
+    void kset_init(struct kset *kset);
+    int kset_add(struct kset *kset);
+    int kset_register(struct kset *kset);
+    void kset_unregister(struct kset *kset);
+• To manage the reference counts of ksets, the situation is about the same:
+    struct kset *kset_get(struct kset *kset);
+    void kset_put(struct kset *kset);
+• A kset also has a name, which is stored in the embedded kobject. So, if you have a kset called my_set , you would set its name with:
+    kobject_set_name(&amp;my_set-&gt;kobj, "The name");
+• Ksets also have a pointer (in the ktype field) to the kobj_type structure describing the kobjects it contains.
+• This type is used in preference to the ktype field in a kobject itself. As a result, in typical usage, the ktype field in struct kobject is left NULL, because the same field within the kset is the one actually used.
+</t>
+  </si>
+  <si>
+    <t>Subsystems</t>
+  </si>
+  <si>
+    <t>
+• A subsystem is a representation for a high-level portion of the kernel as a whole.
+• Sub-systems usually (but not always) show up at the top of the sysfs hierarchy. Some example subsystems in the kernel include block_subsys (/sys/block, for block devices)
+• A subsystem, thus, is really just a wrapper around a kset, with a semaphore thrown in. Every kset must belong to a subsystem.
+• the subsystem’s rwsem semaphore is used to serialize access to a kset’s internal-linked list.
+</t>
+  </si>
+  <si>
+    <t>
+A subsystem is represented by a simple structure:
+    struct subsystem {
+        struct kset kset;
+        struct rw_semaphore rwsem;
+    };
+</t>
+  </si>
+  <si>
+    <t>Low-Level Sysfs Operations</t>
+  </si>
+  <si>
+    <t>
+• Kobjects are the mechanism behind the sysfs virtual filesystem.
+• Every kobject of interest also exports one or more attributes, which appear in that kobject’s sysfs directory as files containing kernel-generated information.
+• Getting a kobject to show up in sysfs is simply a matter of calling kobject_add.
+• There are a couple of things worth knowing about how the sysfs entry is created:
+    - Sysfs entries for kobjects are always directories, so a call to kobject_add results in the creation of a directory in sysfs. Usually that directory contains one or more attributes.
+    - The name assigned to the kobject (with kobject_set_name) is the name used for the sysfs directory. Names assigned to kobjects should also be reasonable file names: they cannot contain the slash character, and the use of white space is strongly discouraged.
+    - The sysfs entry is located in the directory corresponding to the kobject’s parent pointer. 
+    - If parent is NULL when kobject_add is called, it is set to the kobject embedded in the new kobject’s kset; thus, the sysfs hierarchy usually matches the internal hierarchy created with ksets. 
+    - If both parent and kset are NULL , the sysfs directory is created at the top level, which is almost certainly not what you want.
+</t>
+  </si>
+  <si>
+    <t>Default attrubutes</t>
+  </si>
+  <si>
+    <t>
+• When created, every kobject is given a set of default attributes. 
+• These attributes are specified by way of the kobj_type structure. That structure, remember, looks like this:
+• The default_attrs field lists the attributes to be created for every kobject of this type, and sysfs_ops provides the methods to implement those attributes.
+• default_attrs , which points to an array of pointers to attribute structures:
+• In attribute structure, 
+    - name is the name of the attribute (as it appears within the kobject’s sysfs directory), 
+    - owner is a pointer to the module (if any) that is responsible for the implementation of this attribute, and 
+    - mode is the protection bits that are to be applied to this attribute. The mode is usually S_IRUGO for read-only attributes.
+    - modes are defined in &lt;linux/stat.h&gt;).
+• The default_attrs array says what the attributes are but does not tell sysfs how to actually implement those attributes. That task falls to the kobj_type-&gt;sysfs_ops field, which points to a structure defined as:
+• Whenever an attribute is read from user space, the show method is called with a pointer to the kobject and the appropriate attribute structure.
+• That method should encode the value of the given attribute into buffer , being sure not to overrun it (it is PAGE_SIZE bytes), and return the actual length of the returned data.
+• The store method is similar; it should decode the data stored in buffer ( size contains the length of that data, which does not exceed PAGE_SIZE ), store and respond to the new value in whatever way makes sense, and return the number of bytes actually decoded.
+• The store method can be called only if the attribute’s permissions allow writes.
+• If the incoming data does not match expectations, return a negative error value rather than possibly doing something unwanted and unrecoverable.
+</t>
+  </si>
+  <si>
+    <t>
+struct sysfs_ops {
+    ssize_t (*show)(struct kobject *kobj, struct attribute *attr,
+    char *buffer);
+    ssize_t (*store)(struct kobject *kobj, struct attribute *attr,
+    const char *buffer, size_t size);
+};
+struct kobj_type {
+    void (*release)(struct kobject *);
+    struct sysfs_ops *sysfs_ops;
+    struct attribute **default_attrs;
+};
+struct attribute {
+    char *name;
+    struct module *owner;
+    mode_t mode;
+};
+</t>
+  </si>
+  <si>
+    <t>Nondefault Attributes</t>
+  </si>
+  <si>
+    <t>
+• In many cases, the kobject type’s default_attrs field describes all the attributes that kobject will ever have. But that’s not a restriction in the design; attributes can be added and removed to kobjects at will. 
+• If you wish to add a new attribute to a kobject’s sysfs directory, simply fill in an attribute structure and pass it to:
+    int sysfs_create_file(struct kobject *kobj, struct attribute *attr);
+    - the file is created with the name given in the attribute structure, and the return value is 0 ; otherwise, the usual negative error code is returned.
+• Note that the same show( ) and store( ) functions are called to implement operations on the new attribute.
+• Before you add a new, nondefault attribute to a kobject, you should take whatever steps are necessary to ensure that those functions know how to implement that attribute.
+• To remove an attribute, call:
+    int sysfs_remove_file(struct kobject *kobj, struct attribute *attr);
+    - After the call, the attribute no longer appears in the kobject’s sysfs entry.
+</t>
+  </si>
+  <si>
+    <t>Binary Attributes</t>
+  </si>
+  <si>
+    <t>
+• The sysfs conventions call for all attributes to contain a single value in a human-readable text format.
+• That said, there is an occasional, rare need for the creation of attributes that can handle larger chunks of binary data.
+• Binary attributes are described with a bin_attribute structure:
+    - Here, attr is an attribute structure giving the name, owner, and permissions for the binary attribute, 
+    - size is the maximum size of the binary attribute (or 0 if there is no maximum). 
+    - The read and write methods work similarly to the normal char driver equivalents.
+• Binary attributes must be created explicitly; they cannot be set up as default attributes. 
+</t>
+  </si>
+  <si>
+    <t>
+struct bin_attribute {
+    struct attribute attr;
+    size_t size;
+    ssize_t (*read)(struct kobject *kobj, char *buffer, loff_t pos, size_t size);
+    ssize_t (*write)(struct kobject *kobj, char *buffer, loff_t pos, size_t size);
+};
+To create a binary attribute, call:
+    int sysfs_create_bin_file(struct kobject *kobj, struct bin_attribute *attr);
+Binary attributes can be removed with:
+    int sysfs_remove_bin_file(struct kobject *kobj, struct bin_attribute *attr);
+</t>
+  </si>
+  <si>
+    <t>Symbolic Links</t>
+  </si>
+  <si>
+    <t>
+• The link persists even if target is removed from the system. 
+• If you are creating symbolic links to other kobjects, you should probably have a way of knowing about changes to those kobjects, or some sort of assurance that the target kobjects will not disappear.
+</t>
+  </si>
+  <si>
+    <t>
+Creating a symbolic link within sysfs is easy:
+    int sysfs_create_link(struct kobject *kobj, struct kobject *target, char *name);
+Symbolic links can be removed with:
+    void sysfs_remove_link(struct kobject *kobj, char *name);
+</t>
+  </si>
+  <si>
+    <t>Hotplug Event Generation</t>
+  </si>
+  <si>
+    <t>
+• A hotplug event is a notification to user space from the kernel that something has changed in the system’s configuration. They are generated whenever a kobject is created or destroyed.
+• Such events are generated, for example, when a digital camera is plugged in with a USB cable, when a user switches console modes, or when a disk is repartitioned. Hotplug events turn into an invocation of /sbin/hotplug, which can respond to each event by loading drivers, creating device nodes, mounting partitions, or taking any other action that is appropriate.
+• The last major kobject function we look at is the generation of these events. The actual event generation takes place when a kobject is passed to kobject_add or kobject_del. 
+• Before the event is handed to user space, code associated with the kobject (or, more specifically, the kset to which it belongs) has the opportunity to add information for user space or to disable event generation entirely.
+</t>
   </si>
 </sst>
 </file>
@@ -8031,7 +8329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -8128,25 +8426,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -8402,11 +8681,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -13246,10 +13525,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13476,7 +13755,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="562.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="517.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="38" t="s">
         <v>681</v>
       </c>
@@ -13488,7 +13767,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="497.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="468.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="38" t="s">
         <v>684</v>
       </c>
@@ -13842,8 +14121,143 @@
       <c r="D65" s="38" t="s">
         <v>772</v>
       </c>
-      <c r="E65" s="45" t="s">
+      <c r="E65" s="37" t="s">
         <v>773</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="112.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="38" t="s">
+        <v>774</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="247.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="38" t="s">
+        <v>776</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="173.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="38" t="s">
+        <v>778</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="222.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="38" t="s">
+        <v>780</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="186.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="38" t="s">
+        <v>782</v>
+      </c>
+      <c r="D70" s="38" t="s">
+        <v>783</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="100.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="38" t="s">
+        <v>785</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="284.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="38" t="s">
+        <v>787</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="235.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="38" t="s">
+        <v>789</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="100.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="38" t="s">
+        <v>791</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>792</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="222.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C75" s="38" t="s">
+        <v>794</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="345.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C76" s="38" t="s">
+        <v>796</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>797</v>
+      </c>
+      <c r="E76" s="38" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="210.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="38" t="s">
+        <v>799</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="38" t="s">
+        <v>801</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>802</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="75.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="38" t="s">
+        <v>804</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>805</v>
+      </c>
+      <c r="E79" s="45" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="161.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="38" t="s">
+        <v>807</v>
+      </c>
+      <c r="D80" s="38" t="s">
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ldd: linux device model
</commit_message>
<xml_diff>
--- a/short_notes.xlsx
+++ b/short_notes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="864">
   <si>
     <t>Sr No</t>
   </si>
@@ -8478,6 +8478,938 @@
 This call creates an attribute file (/sys/bus/ldd/version) containing the revision number for the lddbus code.
 </t>
   </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>
+• At the lowest level, every device in a Linux system is represented by an instance of struct device :
+struct device *parent
+    The device’s “parent” device—the device to which it is attached. In most cases, a parent device is some sort of bus or host controller. If parent is NULL , the device is a top-level device, which is not usually what you want.
+struct kobject kobj;
+    The kobject that represents this device and links it into the hierarchy. Note that, as a general rule, device-&gt;kobj-&gt;parent is equal to &amp;device-&gt;parent-&gt;kobj .
+char bus_id[BUS_ID_SIZE];
+    A string that uniquely identifies this device on the bus. PCI devices, for example, use the standard PCI ID format containing the domain, bus, device, and function numbers.
+struct bus_type *bus;
+    Identifies which kind of bus the device sits on.
+struct device_driver *driver;
+    The driver that manages this device.
+void *driver_data;
+    A private data field that may be used by the device driver.
+void (*release)(struct device *dev);
+    The method is called when the last reference to the device is removed; it is called from the embedded kobject’s release method. All device structures registered with the core must have a release method, or the kernel prints out scary complaints. At a minimum, the parent , bus_id , bus , and release fields must be set before the device structure can be registered.
+• At a minimum, the parent , bus_id , bus , and release fields must be set before the device structure can be registered.
+</t>
+  </si>
+  <si>
+    <t>
+struct device {
+    struct device *parent;
+    struct kobject kobj;
+    char bus_id[BUS_ID_SIZE];
+    struct bus_type *bus;
+    struct device_driver *driver;
+    void *driver_data;
+    void (*release)(struct device *dev);
+    /* Several fields omitted */
+};
+</t>
+  </si>
+  <si>
+    <t>Device registration</t>
+  </si>
+  <si>
+    <t>
+• The usual set of registration and unregistration functions exists:
+    int device_register(struct device *dev);
+    void device_unregister(struct device *dev);
+• We have seen how the lddbus code registers its bus type. However, an actual bus is a device and must be registered separately.
+</t>
+  </si>
+  <si>
+    <t>
+static void ldd_bus_release(struct device *dev) {
+    printk(KERN_DEBUG "lddbus release\n");
+}
+struct device ldd_bus = {
+    .bus_id = "ldd0",
+    .release = ldd_bus_release
+};
+This is a top-level bus, so the parent and bus fields are left NULL . We have a simple, no-op release method, and, as the first (and only) bus, its name is ldd0 . This bus device is registered with:
+ret = device_register(&amp;ldd_bus);
+    if (ret)
+        printk(KERN_NOTICE "Unable to register ldd0\n");
+Once that call is complete, the new bus can be seen under /sys/devices in sysfs. Any devices added to this bus then shows up under /sys/devices/ldd0/.
+</t>
+  </si>
+  <si>
+    <t>Device attributes</t>
+  </si>
+  <si>
+    <t>
+• Device entries in sysfs can have attributes. The relevant structure is:
+• These attribute structures can be set up at compile time with this macro:
+    DEVICE_ATTR(name, mode, show, store);
+    - The resulting structure is named by prepending dev_attr_ to the given name . 
+• The actual management of attribute files is handled with the usual pair of functions:
+int device_create_file(struct device *device, struct device_attribute *entry);
+void device_remove_file(struct device *dev, struct device_attribute *attr);
+    The dev_attrs field of struct bus_type points to a list of default attributes created for every device added to that bus.
+</t>
+  </si>
+  <si>
+    <t>
+struct device_attribute {
+    struct attribute attr;
+    ssize_t (*show)(struct device *dev, char *buf);
+    ssize_t (*store)(struct device *dev, const char *buf, size_t count);
+};
+</t>
+  </si>
+  <si>
+    <t>Device structure embedding</t>
+  </si>
+  <si>
+    <t>
+• The device structure contains the information that the device model core needs to model the system. Most subsystems, however, track additional information about the devices they host. 
+• As a result, it is rare for devices to be represented by bare device structures; instead, that structure, like kobject structures, is usually embedded within a higher-level representation of the device. 
+• If you look at the definitions of struct pci_dev or struct usb_device , you will find a struct device buried inside.
+• Usually, low-level drivers are not even aware of that struct device , but there can be exceptions.
+• The lddbus driver creates its own device type ( struct ldd_device ) and expects individual device drivers to register their devices using that type.
+• It is a simple structure struct ldd_device:
+    - This structure allows the driver to provide an actual name for the device (which can be distinct from its bus ID, stored in the device structure) and a pointer to driver information. Structures for real devices usually also contain information about the vendor, device model, device configuration, resources used, and so on.
+    - Good examples can be found in struct pci_dev (&lt;linux/pci.h&gt;) or struct usb_device (&lt;linux/usb.h&gt;). 
+    - A convenience macro (to_ldd_device) is also defined for struct ldd_device to make it easy to turn pointers to the embedded device structure into ldd_device pointers.
+• The registration interface exported by lddbus looks like register_ldd_device ():
+• Here, we simply fill in some of the embedded device structure fields (which individual drivers should not need to know about), and register the device with the driver core. 
+• If we wanted to add bus-specific attributes to the device, we could do so here.
+</t>
+  </si>
+  <si>
+    <t>
+struct ldd_device {
+    char *name;
+    struct ldd_driver *driver;
+    struct device dev;
+};
+#define to_ldd_device(dev) container_of(dev, struct ldd_device, dev);
+int register_ldd_device(struct ldd_device *ldddev) {
+    ldddev-&gt;dev.bus = &amp;ldd_bus_type;
+    ldddev-&gt;dev.parent = &amp;ldd_bus;
+    ldddev-&gt;dev.release = ldd_dev_release;
+    strncpy(ldddev-&gt;dev.bus_id, ldddev-&gt;name, BUS_ID_SIZE);
+    return device_register(&amp;ldddev-&gt;dev);
+}
+EXPORT_SYMBOL(register_ldd_device);
+To show how this interface is used, let us introduce another sample driver, which we have called sculld.
+</t>
+  </si>
+  <si>
+    <t>Device Driver</t>
+  </si>
+  <si>
+    <t>
+• The device model tracks all of the drivers known to the system. The main reason for this tracking is to enable the driver core to match up drivers with new devices. 
+• Once drivers are known objects within the system, however, a number of other things become possible. 
+• Device drivers can export information and configuration variables that are independent of any specific device, for example.
+• Drivers are defined by the structure struct device_driver:
+    - name is the name of the driver (it shows up in sysfs), 
+    - bus is the type of bus this driver works with, 
+    - kobj is the inevitable kobject, 
+    - devices is a list of all devices currently bound to this driver, 
+    - probe is a function called to query the existence of a specific device (and whether this driver can work with it), 
+    - remove is called when the device is removed from the system, and shutdown is called at shutdown time to quiesce the device.
+• The registration functions are:
+    int driver_register(struct device_driver *drv);
+    void driver_unregister(struct device_driver *drv);
+• The usual attribute structure struct driver_attribute:
+• And attribute files are created in the usual way:
+    int driver_create_file(struct device_driver *drv, struct driver_attribute *attr);
+    void driver_remove_file(struct device_driver *drv, struct driver_attribute *attr);
+• The bus_type structure contains a field ( drv_attrs ) that points to a set of default attributes, which are created for all drivers associated with that bus.
+</t>
+  </si>
+  <si>
+    <t>
+struct device_driver {
+    char *name;
+    struct bus_type *bus;
+    struct kobject kobj;
+    struct list_head devices;
+    int (*probe)(struct device *dev);
+    int (*remove)(struct device *dev);
+    void (*shutdown) (struct device *dev);
+};
+several of the structure’s fields have been omitted (see &lt;linux/device.h&gt;).
+struct driver_attribute {
+    struct attribute attr;
+    ssize_t (*show)(struct device_driver *drv, char *buf);
+    ssize_t (*store)(struct device_driver *drv, const char *buf, size_t count);
+};
+DRIVER_ATTR(name, mode, show, store);
+</t>
+  </si>
+  <si>
+    <t>Driver structure embedding</t>
+  </si>
+  <si>
+    <t>
+• As is the case with most driver core structures, the device_driver structure is usually found embedded within a higher-level, bus-specific structure.
+• The lddbus subsystem would never go against such a trend, so it has defined its own ldd_driver structure struct ldd_driver:
+    - Here, we require each driver to provide its current software version, and lddbus exports that version string for every driver it knows about. 
+• The bus-specific driver registration function register_ldd_driver ():
+    - The first half of the function simply registers the low-level device_driver structure with the core; the rest sets up the version attribute. 
+    - Since this attribute is created atruntime, we can’t use the DRIVER_ATTR macro; instead, the driver_attribute structure must be filled in by hand.
+    - Note that we set the owner of the attribute to the driver module, rather than the lddbus module; the reason for this can be seen in the implementation of the show function for this attribute:
+</t>
+  </si>
+  <si>
+    <t>
+struct ldd_driver {
+    char *version;
+    struct module *module;
+    struct device_driver driver;
+    struct driver_attribute version_attr;
+};
+#define to_ldd_driver(drv) container_of(drv, struct ldd_driver, driver);
+int register_ldd_driver(struct ldd_driver *driver) {
+    int ret;
+    driver-&gt;driver.bus = &amp;ldd_bus_type;
+    ret = driver_register(&amp;driver-&gt;driver);
+    if (ret)
+    return ret;
+    driver-&gt;version_attr.attr.name = "version";
+    driver-&gt;version_attr.attr.owner = driver-&gt;module;
+    driver-&gt;version_attr.attr.mode = S_IRUGO;
+    driver-&gt;version_attr.show = show_version;
+    driver-&gt;version_attr.store = NULL;
+    return driver_create_file(&amp;driver-&gt;driver, &amp;driver-&gt;version_attr);
+}
+static ssize_t show_version(struct device_driver *driver, char *buf) {
+    struct ldd_driver *ldriver = to_ldd_driver(driver);
+    sprintf(buf, "%s\n", ldriver-&gt;version);
+    return strlen(buf);
+}
+For completeness, sculld creates its ldd_driver structure as follows:
+static struct ldd_driver sculld_driver = {
+    .version = "$Revision: 1.1 $",
+    .module = THIS_MODULE,
+    .driver = {.name = "sculld",},
+};
+A simple call to register_ldd_driver adds it to the system. Once initialization is complete, the driver information can be seen in sysfs:
+$ tree /sys/bus/ldd/drivers
+</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>
+• A class is a higher-level view of a device that abstracts out low-level implementation details.
+• Drivers may see a SCSI disk or an ATA disk, but, at the class level, they are all simply disks. 
+• Classes allow user space to work with devices based on what they do, rather than how they are connected or how they work.
+• Almost all classes show up in sysfs under /sys/class.
+• The one exception is block devices, which can be found under /sys/block for historical reasons.
+• Class membership is usually handled by high-level code without the need for explicit support from drivers.
+</t>
+  </si>
+  <si>
+    <t>The class_simple Interface</t>
+  </si>
+  <si>
+    <t>
+• To create and destroy class class_simple_create () and class_simple_destroy () resp.:
+    - class_simple_create () function creates a class with the given name .
+• The real purpose of creating a simple class is to add devices to it; that task is achieved with class_simple_device_add ():
+    - cs is the previously created simple class, 
+    - devnum is the assigned device number,
+    - device is the struct device representing this device
+    - the remaining parameters are a printk-style format string and arguments to create the device name. 
+    - This call adds an entry to the class containing one attribute, dev , which holds the device number. 
+    - If the device parameter is not NULL , a symbolic link (called device ) points to the device’s entry under /sys/devices.
+• It is possible to add other attributes to a device entry. It is just a matter of using class_device_create_file,
+• Classes generate hotplug events when devices come and go. If your driver needs to add variables to the environment for the user-space event handler, it can set up a hotplug callback with:
+    int class_simple_set_hotplug(struct class_simple *cs, int (*hotplug)(struct class_device *dev, char **envp, int num_envp, char *buffer, int buffer_size));
+• When your device goes away, the class entry should be removed with class_simple_device_remove ():
+    - Note that the class_device structure returned by class_simple_device_add is not needed here; the device number (which should certainly be unique) is sufficient.
+</t>
+  </si>
+  <si>
+    <r>
+      <t>
+struct class_simple *class_simple_create(struct module *owner, char *name);
+void class_simple_destroy(struct class_simple *cs);
+struct class_device *class_simple_device_add(struct class_simple *cs, dev_t devnum,struct device *device,const char *fmt, ...);
+void class_simple_device_remove(dev_t dev);
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Managing classes</t>
+  </si>
+  <si>
+    <t>
+• A class is defined by an instance of struct class :
+    - Each class needs a unique name , which is how this class appears under /sys/class. When the class is registered, 
+    - all of the attributes listed in the ( NULL -terminated) array pointed to by class_attrs is created. 
+    - There is also a set of default attributes for every device added to the class; class_dev_attrs points to those. 
+    - There is the usual hotplug function for adding variables to the environment when events are generated.
+    - There are also two release methods: release is called whenever a device is removed from the class, while class_release is called when the class itself is released.
+• The registration functions are:
+int class_register(struct class *cls);
+void class_unregister(struct class *cls);
+• The interface for working with attributes should not surprise anybody at this point:
+</t>
+  </si>
+  <si>
+    <t>
+struct class {
+    char *name;
+    struct class_attribute *class_attrs;
+    struct class_device_attribute *class_dev_attrs;
+    int (*hotplug)(struct class_device *dev, char **envp,
+    int num_envp, char *buffer, int buffer_size);
+    void (*release)(struct class_device *dev);
+    void (*class_release)(struct class *class);
+    /* Some fields omitted */
+};
+struct class_attribute {
+    struct attribute attr;
+    ssize_t (*show)(struct class *cls, char *buf);
+    ssize_t (*store)(struct class *cls, const char *buf, size_t count);
+};
+CLASS_ATTR(name, mode, show, store);
+int class_create_file(struct class *cls, const struct class_attribute *attr);
+void class_remove_file(struct class *cls, const struct class_attribute *attr);
+</t>
+  </si>
+  <si>
+    <t>Class devices</t>
+  </si>
+  <si>
+    <t>
+• The real purpose of a class is to serve as a container for the devices that are members of that class. A member is represented by struct class_device :
+    - The class_id field holds the name of this device as it appears in sysfs. 
+    - The class pointer should point to the class holding this device, and 
+    - dev should point to the associated device structure. Setting dev is optional; if it is non- NULL , it is used to create a symbolic link from the class entry to the corresponding entry under /sys/devices, making it easy to find the device entry in user space. 
+    - The class can use class_data to hold a private pointer.
+• The class device interface also allows the renaming of an already registered entry:
+    int class_device_rename(struct class_device *cd, char *new_name);
+• Class device entries have attributes:
+</t>
+  </si>
+  <si>
+    <t>
+struct class_device {
+    struct kobject kobj;
+    struct class *class;
+    struct device *dev;
+    void *class_data;
+    char class_id[BUS_ID_SIZE];
+};
+int class_device_register(struct class_device *cd);
+void class_device_unregister(struct class_device *cd);
+struct class_device_attribute {
+    struct attribute attr;
+    ssize_t (*show)(struct class_device *cls, char *buf);
+    ssize_t (*store)(struct class_device *cls, const char *buf,
+    size_t count);
+};
+</t>
+  </si>
+  <si>
+    <t>Class interfaces</t>
+  </si>
+  <si>
+    <t>
+• The class subsystem has an additional concept not found in other parts of the Linux device model. This mechanism is called an interface, but it is, perhaps, best thought of as a sort of trigger mechanism that can be used to get notification when devices enter or leave the class.
+• The functioning of an interface is straightforward. Whenever a class device is added to the class specified in the class_interface structure, the interface’s add function is called. 
+• That function can perform any additional setup required for that device; this setup often takes the form of adding more attributes, but other applications are possible.
+• When the device is removed from the class, the remove method is called to perform any required cleanup.
+• Multiple interfaces can be registered for a class.
+</t>
+  </si>
+  <si>
+    <t>
+struct class_interface {
+    struct class *class;
+    int (*add) (struct class_device *cd);
+    void (*remove) (struct class_device *cd);
+};
+int class_interface_register(struct class_interface *intf);
+void class_interface_unregister(struct class_interface *intf);
+</t>
+  </si>
+  <si>
+    <t>Quick Reference</t>
+  </si>
+  <si>
+    <r>
+      <t>    
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Kobjects
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>#include &lt;linux/kobject.h&gt;
+The include file containing definitions for kobjects, related structures, and functions.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>void kobject_init(struct kobject *kobj);
+int kobject_set_name(struct kobject *kobj, const char *format, ...);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions for kobject initialization.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>struct kobject *kobject_get(struct kobject *kobj);
+void kobject_put(struct kobject *kobj);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that manage reference counts for kobjects.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>struct kobj_type;
+struct kobj_type *get_ktype(struct kobject *kobj);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Represents the type of structure within which a kobject is embedded. Use get_ktype to get the kobj_type associated with a given kobject.
+i</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>nt kobject_add(struct kobject *kobj);
+extern int kobject_register(struct kobject *kobj);
+void kobject_del(struct kobject *kobj);
+void kobject_unregister(struct kobject *kobj);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   kobject_add adds a kobject to the system, handling kset membership, sysfs repre sentation, and hotplug event generation. kobject_register is a convenience function that combines kobject_init and kobject_add. Use kobject_del to remove a kobject or kobject_unregister, which combines kobject_del and kobject_put.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>void kset_init(struct kset *kset);
+int kset_add(struct kset *kset);
+int kset_register(struct kset *kset);
+void kset_unregister(struct kset *kset);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Initialization and registration functions for ksets.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Decl_subsys(name, type, hotplug_ops);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   A macro that makes it easier to declare subsystems.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>void subsystem_init(struct subsystem *subsys);
+int subsystem_register(struct subsystem *subsys);
+void subsystem_unregister(struct subsystem *subsys);
+struct subsystem *subsys_get(struct subsystem *subsys)
+void subsys_put(struct subsystem *subsys);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Operations on subsystems.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sysfs Operations
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>#include &lt;linux/sysfs.h&gt;
+The include file containing declarations for sysfs.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int sysfs_create_file(struct kobject *kobj, struct attribute *attr);
+int sysfs_remove_file(struct kobject *kobj, struct attribute *attr);
+int sysfs_create_bin_file(struct kobject *kobj, struct bin_attribute *attr);
+int sysfs_remove_bin_file(struct kobject *kobj, struct bin_attribute *attr);
+int sysfs_create_link(struct kobject *kobj, struct kobject *target, char *name);
+void sysfs_remove_link(struct kobject *kobj, char *name);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions for creating and removing attribute files associated with a kobject.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Firmware
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>#include &lt;linux/firmware.h&gt;
+i</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>nt request_firmware(const struct firmware **fw, char *name, struct device *device);
+int request_firmware_nowait(struct module *module, char *name, struct device
+*device, void *context, void (*cont)(const struct firmware *fw, void *context));
+void release_firmware(struct firmware *fw);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that implement the kernel firmware-loading interface.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Buses, Devices, and Drivers
+int bus_register(struct bus_type *bus);
+void bus_unregister(struct bus_type *bus);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that perform registration and unregistration of buses in the device model.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int bus_for_each_dev(struct bus_type *bus, struct device *start, void *data,
+int (*fn)(struct device *, void *));
+int bus_for_each_drv(struct bus_type *bus, struct device_driver *start, void *data, int (*fn)(struct device_driver *, void *));
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that iterate over each of the devices and drivers, respectively, that are attached to the given bus.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>BUS_ATTR(name, mode, show, store);
+int bus_create_file(struct bus_type *bus, struct bus_attribute *attr);
+void bus_remove_file(struct bus_type *bus, struct bus_attribute *attr);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   The BUS_ATTR macro may be used to declare a bus_attribute structure, which may then be added and removed with the above two functions.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int device_register(struct device *dev);
+void device_unregister(struct device *dev);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that handle device registration.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>DEVICE_ATTR(name, mode, show, store);
+int device_create_file(struct device *device, struct device_attribute *entry);
+void device_remove_file(struct device *dev, struct device_attribute *attr);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Macros and functions that deal with device attributes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int driver_register(struct device_driver *drv);
+void driver_unregister(struct device_driver *drv);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that register and unregister a device driver.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>DRIVER_ATTR(name, mode, show, store);
+int driver_create_file(struct device_driver *drv, struct driver_attribute *attr);
+void driver_remove_file(struct device_driver *drv, struct driver_attribute *attr);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Macros and functions that manage driver attributes.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Classes
+struct class_simple *class_simple_create(struct module *owner, char *name);
+void class_simple_destroy(struct class_simple *cs);
+struct class_device *class_simple_device_add(struct class_simple *cs, dev_t
+devnum, struct device *device, const char *fmt, ...);
+void class_simple_device_remove(dev_t dev);
+int class_simple_set_hotplug(struct class_simple *cs, int (*hotplug)(structclass_device *dev, char **envp, int num_envp, char *buffer, int buffer_size));
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that implement the class_simple interface; they manage simple class entries containing a dev attribute and little else.
+i</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>nt class_register(struct class *cls);
+void class_unregister(struct class *cls);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>    Registration and unregistration of classes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>CLASS_ATTR(name, mode, show, store);
+int class_create_file(struct class *cls, const struct class_attribute *attr);
+void class_remove_file(struct class *cls, const struct class_attribute *attr);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>    The usual macros and functions for dealing with class attributes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int class_device_register(struct class_device *cd);
+void class_device_unregister(struct class_device *cd);
+int class_device_rename(struct class_device *cd, char *new_name);
+CLASS_DEVICE_ATTR(name, mode, show, store);
+Int class_device_create_file(struct class_device *cls, const struct class_device_attribute *attr);
+void class_device_remove_file(struct class_device *cls, const struct class_device_attribute *attr);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>    Functions and macros that implement the class device interface.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>int class_interface_register(struct class_interface *intf);
+void class_interface_unregister(struct class_interface *intf);
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>   Functions that add an interface to a class (or remove it).
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -8486,7 +9418,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -8582,6 +9514,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -8656,7 +9593,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -8834,6 +9771,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -13673,10 +14614,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D87" activeCellId="0" sqref="D87"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A99" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14474,6 +15415,143 @@
         <v>826</v>
       </c>
     </row>
+    <row r="87" customFormat="false" ht="333.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="38" t="s">
+        <v>827</v>
+      </c>
+      <c r="D87" s="38" t="s">
+        <v>828</v>
+      </c>
+      <c r="E87" s="45" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="210.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="38" t="s">
+        <v>830</v>
+      </c>
+      <c r="D88" s="38" t="s">
+        <v>831</v>
+      </c>
+      <c r="E88" s="38" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="136.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="38" t="s">
+        <v>833</v>
+      </c>
+      <c r="D89" s="38" t="s">
+        <v>834</v>
+      </c>
+      <c r="E89" s="45" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="321.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="D90" s="38" t="s">
+        <v>837</v>
+      </c>
+      <c r="E90" s="38" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="321.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="38" t="s">
+        <v>839</v>
+      </c>
+      <c r="D91" s="38" t="s">
+        <v>840</v>
+      </c>
+      <c r="E91" s="38" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="493.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="38" t="s">
+        <v>842</v>
+      </c>
+      <c r="D92" s="38" t="s">
+        <v>843</v>
+      </c>
+      <c r="E92" s="38" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="136.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="38" t="s">
+        <v>845</v>
+      </c>
+      <c r="D93" s="38" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="321.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="38" t="s">
+        <v>847</v>
+      </c>
+      <c r="D94" s="38" t="s">
+        <v>848</v>
+      </c>
+      <c r="E94" s="38" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="259.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="45" t="s">
+        <v>850</v>
+      </c>
+      <c r="D95" s="38" t="s">
+        <v>851</v>
+      </c>
+      <c r="E95" s="38" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="235.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="37" t="s">
+        <v>853</v>
+      </c>
+      <c r="D96" s="38" t="s">
+        <v>854</v>
+      </c>
+      <c r="E96" s="38" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="38" t="s">
+        <v>856</v>
+      </c>
+      <c r="D97" s="38" t="s">
+        <v>857</v>
+      </c>
+      <c r="E97" s="38" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="38" t="s">
+        <v>859</v>
+      </c>
+      <c r="D98" s="38" t="s">
+        <v>860</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="431.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D99" s="38" t="s">
+        <v>862</v>
+      </c>
+      <c r="E99" s="38" t="s">
+        <v>863</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>